<commit_message>
Created folder of sets for each faction. Each faction will ideally have set for Creatures, Champions, Spells, Artifacts/Enchantments, Lands, etc.
</commit_message>
<xml_diff>
--- a/DesignDoc.xlsx
+++ b/DesignDoc.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="488">
   <si>
     <t>Description</t>
   </si>
@@ -1546,6 +1546,29 @@
   </si>
   <si>
     <t>Moon Shadow Titan</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> These are just ideas for names.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2628,7 +2651,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="198">
+  <cellXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3094,96 +3117,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3194,6 +3136,90 @@
     <xf numFmtId="0" fontId="1" fillId="33" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3212,8 +3238,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3962,7 +3988,7 @@
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="156"/>
       <c r="B19" s="156"/>
-      <c r="C19" s="197" t="s">
+      <c r="C19" s="157" t="s">
         <v>476</v>
       </c>
       <c r="D19" s="156"/>
@@ -4517,10 +4543,10 @@
       <c r="F25" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="I25" s="157" t="s">
+      <c r="I25" s="158" t="s">
         <v>370</v>
       </c>
-      <c r="J25" s="157"/>
+      <c r="J25" s="158"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
@@ -4538,8 +4564,8 @@
       <c r="F26" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="I26" s="158"/>
-      <c r="J26" s="158"/>
+      <c r="I26" s="159"/>
+      <c r="J26" s="159"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="12" t="s">
@@ -4731,10 +4757,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:O39"/>
+  <dimension ref="B2:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4744,510 +4770,500 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1"/>
-      <c r="C1"/>
-      <c r="D1"/>
-      <c r="E1"/>
-      <c r="F1"/>
-    </row>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="163" t="s">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="198" t="s">
+        <v>487</v>
+      </c>
+      <c r="C2" s="198"/>
+    </row>
+    <row r="3" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="182" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="164"/>
-      <c r="D2" s="165" t="s">
+      <c r="C5" s="183"/>
+      <c r="D5" s="184" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="166"/>
-      <c r="F2" s="167" t="s">
+      <c r="E5" s="185"/>
+      <c r="F5" s="186" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="168"/>
-      <c r="H2" s="169" t="s">
+      <c r="G5" s="187"/>
+      <c r="H5" s="188" t="s">
         <v>382</v>
       </c>
-      <c r="I2" s="170"/>
-      <c r="J2" s="171" t="s">
+      <c r="I5" s="189"/>
+      <c r="J5" s="190" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="172"/>
-    </row>
-    <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="39" t="s">
+      <c r="K5" s="191"/>
+    </row>
+    <row r="6" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C6" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D6" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E6" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F6" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="G6" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="45" t="s">
+      <c r="H6" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="46" t="s">
+      <c r="I6" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="47" t="s">
+      <c r="J6" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="40" t="s">
+      <c r="K6" s="40" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="48" t="s">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="48" t="s">
         <v>208</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C7" s="60" t="s">
         <v>209</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D7" s="48" t="s">
         <v>210</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E7" s="49" t="s">
         <v>473</v>
       </c>
-      <c r="F4" s="62" t="s">
+      <c r="F7" s="62" t="s">
         <v>211</v>
       </c>
-      <c r="G4" s="60" t="s">
+      <c r="G7" s="60" t="s">
         <v>212</v>
       </c>
-      <c r="H4" s="48" t="s">
+      <c r="H7" s="48" t="s">
         <v>213</v>
       </c>
-      <c r="I4" s="49" t="s">
+      <c r="I7" s="49" t="s">
         <v>214</v>
       </c>
-      <c r="J4" s="62" t="s">
+      <c r="J7" s="62" t="s">
         <v>215</v>
       </c>
-      <c r="K4" s="49" t="s">
+      <c r="K7" s="49" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="33" t="s">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="33" t="s">
         <v>217</v>
       </c>
-      <c r="C5" s="61" t="s">
+      <c r="C8" s="61" t="s">
         <v>218</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D8" s="33" t="s">
         <v>219</v>
       </c>
-      <c r="E5" s="34" t="s">
+      <c r="E8" s="34" t="s">
         <v>220</v>
       </c>
-      <c r="F5" s="63" t="s">
+      <c r="F8" s="63" t="s">
         <v>221</v>
       </c>
-      <c r="G5" s="61" t="s">
+      <c r="G8" s="61" t="s">
         <v>222</v>
       </c>
-      <c r="H5" s="33" t="s">
+      <c r="H8" s="33" t="s">
         <v>483</v>
       </c>
-      <c r="I5" s="34" t="s">
+      <c r="I8" s="34" t="s">
         <v>223</v>
       </c>
-      <c r="J5" s="63" t="s">
+      <c r="J8" s="63" t="s">
         <v>224</v>
       </c>
-      <c r="K5" s="34" t="s">
+      <c r="K8" s="34" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="159" t="s">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="164" t="s">
         <v>226</v>
       </c>
-      <c r="C6" s="160"/>
-      <c r="D6" s="159" t="s">
+      <c r="C9" s="166"/>
+      <c r="D9" s="164" t="s">
         <v>472</v>
       </c>
-      <c r="E6" s="161"/>
-      <c r="F6" s="162" t="s">
+      <c r="E9" s="165"/>
+      <c r="F9" s="167" t="s">
         <v>227</v>
       </c>
-      <c r="G6" s="160"/>
-      <c r="H6" s="159" t="s">
+      <c r="G9" s="166"/>
+      <c r="H9" s="164" t="s">
         <v>228</v>
       </c>
-      <c r="I6" s="161"/>
-      <c r="J6" s="162" t="s">
+      <c r="I9" s="165"/>
+      <c r="J9" s="167" t="s">
         <v>229</v>
       </c>
-      <c r="K6" s="161"/>
-      <c r="N6"/>
-    </row>
-    <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="183" t="s">
+      <c r="K9" s="165"/>
+    </row>
+    <row r="10" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="168" t="s">
         <v>230</v>
       </c>
-      <c r="C7" s="184"/>
-      <c r="D7" s="183" t="s">
+      <c r="C10" s="170"/>
+      <c r="D10" s="168" t="s">
         <v>231</v>
       </c>
-      <c r="E7" s="185"/>
-      <c r="F7" s="186" t="s">
+      <c r="E10" s="169"/>
+      <c r="F10" s="171" t="s">
         <v>474</v>
       </c>
-      <c r="G7" s="184"/>
-      <c r="H7" s="183" t="s">
+      <c r="G10" s="170"/>
+      <c r="H10" s="168" t="s">
         <v>468</v>
       </c>
-      <c r="I7" s="185"/>
-      <c r="J7" s="186" t="s">
+      <c r="I10" s="169"/>
+      <c r="J10" s="171" t="s">
         <v>232</v>
       </c>
-      <c r="K7" s="185"/>
-      <c r="N7"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="N8"/>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="N9"/>
-    </row>
-    <row r="10" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="N10"/>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="173" t="s">
+      <c r="K10" s="169"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+    </row>
+    <row r="13" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="172" t="s">
         <v>371</v>
       </c>
-      <c r="C11" s="174"/>
-      <c r="D11" s="175" t="s">
+      <c r="C14" s="173"/>
+      <c r="D14" s="174" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="176"/>
-      <c r="F11" s="177" t="s">
+      <c r="E14" s="175"/>
+      <c r="F14" s="176" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="178"/>
-      <c r="H11" s="179" t="s">
+      <c r="G14" s="177"/>
+      <c r="H14" s="178" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="180"/>
-      <c r="J11" s="181" t="s">
+      <c r="I14" s="179"/>
+      <c r="J14" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="182"/>
-      <c r="N11"/>
-      <c r="O11"/>
-    </row>
-    <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="51" t="s">
+      <c r="K14" s="181"/>
+    </row>
+    <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="52" t="s">
+      <c r="C15" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="53" t="s">
+      <c r="D15" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="54" t="s">
+      <c r="E15" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="55" t="s">
+      <c r="F15" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="56" t="s">
+      <c r="G15" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="57" t="s">
+      <c r="H15" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="I12" s="58" t="s">
+      <c r="I15" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="J12" s="83" t="s">
+      <c r="J15" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="K12" s="59" t="s">
+      <c r="K15" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="N12"/>
-      <c r="O12"/>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="31" t="s">
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="31" t="s">
         <v>388</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C16" s="32" t="s">
         <v>485</v>
       </c>
-      <c r="D13" s="66" t="s">
+      <c r="D16" s="66" t="s">
         <v>236</v>
       </c>
-      <c r="E13" s="32" t="s">
+      <c r="E16" s="32" t="s">
         <v>237</v>
       </c>
-      <c r="F13" s="66" t="s">
+      <c r="F16" s="66" t="s">
         <v>238</v>
       </c>
-      <c r="G13" s="65" t="s">
+      <c r="G16" s="65" t="s">
         <v>239</v>
       </c>
-      <c r="H13" s="31" t="s">
+      <c r="H16" s="31" t="s">
         <v>234</v>
       </c>
-      <c r="I13" s="65" t="s">
+      <c r="I16" s="65" t="s">
         <v>235</v>
       </c>
-      <c r="J13" s="31"/>
-      <c r="K13" s="32" t="s">
+      <c r="J16" s="31"/>
+      <c r="K16" s="32" t="s">
         <v>233</v>
       </c>
-      <c r="N13"/>
-      <c r="O13"/>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="35" t="s">
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="35" t="s">
         <v>249</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C17" s="36" t="s">
         <v>486</v>
       </c>
-      <c r="D14" s="64" t="s">
+      <c r="D17" s="64" t="s">
         <v>243</v>
       </c>
-      <c r="E14" s="34" t="s">
+      <c r="E17" s="34" t="s">
         <v>244</v>
       </c>
-      <c r="F14" s="63" t="s">
+      <c r="F17" s="63" t="s">
         <v>245</v>
       </c>
-      <c r="G14" s="61" t="s">
+      <c r="G17" s="61" t="s">
         <v>246</v>
       </c>
-      <c r="H14" s="33" t="s">
+      <c r="H17" s="33" t="s">
         <v>241</v>
       </c>
-      <c r="I14" s="61" t="s">
+      <c r="I17" s="61" t="s">
         <v>242</v>
       </c>
-      <c r="J14" s="35"/>
-      <c r="K14" s="36" t="s">
+      <c r="J17" s="35"/>
+      <c r="K17" s="36" t="s">
         <v>240</v>
       </c>
-      <c r="N14"/>
-      <c r="O14"/>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="159" t="s">
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="164" t="s">
         <v>484</v>
       </c>
-      <c r="C15" s="161"/>
-      <c r="D15" s="162" t="s">
+      <c r="C18" s="165"/>
+      <c r="D18" s="167" t="s">
         <v>248</v>
       </c>
-      <c r="E15" s="161"/>
-      <c r="F15" s="162" t="s">
+      <c r="E18" s="165"/>
+      <c r="F18" s="167" t="s">
         <v>250</v>
       </c>
-      <c r="G15" s="160"/>
-      <c r="H15" s="159" t="s">
+      <c r="G18" s="166"/>
+      <c r="H18" s="164" t="s">
         <v>247</v>
       </c>
-      <c r="I15" s="160"/>
-      <c r="J15" s="159" t="s">
+      <c r="I18" s="166"/>
+      <c r="J18" s="164" t="s">
         <v>434</v>
       </c>
-      <c r="K15" s="161"/>
-      <c r="N15"/>
-      <c r="O15"/>
-    </row>
-    <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="183" t="s">
+      <c r="K18" s="165"/>
+    </row>
+    <row r="19" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="168" t="s">
         <v>253</v>
       </c>
-      <c r="C16" s="185"/>
-      <c r="D16" s="186" t="s">
+      <c r="C19" s="169"/>
+      <c r="D19" s="171" t="s">
         <v>252</v>
       </c>
-      <c r="E16" s="185"/>
-      <c r="F16" s="186" t="s">
+      <c r="E19" s="169"/>
+      <c r="F19" s="171" t="s">
         <v>254</v>
       </c>
-      <c r="G16" s="184"/>
-      <c r="H16" s="183" t="s">
+      <c r="G19" s="170"/>
+      <c r="H19" s="168" t="s">
         <v>251</v>
       </c>
-      <c r="I16" s="184"/>
-      <c r="J16" s="183" t="s">
+      <c r="I19" s="170"/>
+      <c r="J19" s="168" t="s">
         <v>471</v>
       </c>
-      <c r="K16" s="185"/>
-    </row>
-    <row r="18" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="87" t="s">
+      <c r="K19" s="169"/>
+    </row>
+    <row r="21" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="87" t="s">
         <v>258</v>
       </c>
-      <c r="E19" s="89" t="s">
+      <c r="E22" s="89" t="s">
         <v>255</v>
       </c>
-      <c r="F19" s="93" t="s">
+      <c r="F22" s="93" t="s">
         <v>256</v>
       </c>
-      <c r="G19" s="8"/>
-      <c r="I19" s="188" t="s">
+      <c r="G22" s="8"/>
+      <c r="I22" s="161" t="s">
         <v>257</v>
       </c>
-      <c r="J19" s="189"/>
-      <c r="K19" s="190"/>
-    </row>
-    <row r="20" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="81" t="s">
+      <c r="J22" s="162"/>
+      <c r="K22" s="163"/>
+    </row>
+    <row r="23" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="88" t="s">
+      <c r="E23" s="88" t="s">
         <v>288</v>
       </c>
-      <c r="F20" s="82" t="s">
+      <c r="F23" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="I20" s="84" t="s">
+      <c r="I23" s="84" t="s">
         <v>259</v>
       </c>
-      <c r="J20" s="85" t="s">
+      <c r="J23" s="85" t="s">
         <v>260</v>
       </c>
-      <c r="K20" s="86" t="s">
+      <c r="K23" s="86" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="69" t="s">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="69" t="s">
         <v>475</v>
       </c>
-      <c r="E21" s="31" t="s">
+      <c r="E24" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="F21" s="73" t="s">
+      <c r="F24" s="73" t="s">
         <v>263</v>
       </c>
-      <c r="I21" s="72" t="s">
+      <c r="I24" s="72" t="s">
         <v>264</v>
       </c>
-      <c r="J21" s="77" t="s">
+      <c r="J24" s="77" t="s">
         <v>265</v>
       </c>
-      <c r="K21" s="76" t="s">
+      <c r="K24" s="76" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="70" t="s">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="70" t="s">
         <v>272</v>
       </c>
-      <c r="E22" s="33" t="s">
+      <c r="E25" s="33" t="s">
         <v>267</v>
       </c>
-      <c r="F22" s="74" t="s">
+      <c r="F25" s="74" t="s">
         <v>268</v>
       </c>
-      <c r="I22" s="78" t="s">
+      <c r="I25" s="78" t="s">
         <v>269</v>
       </c>
-      <c r="J22" s="79" t="s">
+      <c r="J25" s="79" t="s">
         <v>270</v>
       </c>
-      <c r="K22" s="9" t="s">
+      <c r="K25" s="9" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="70" t="s">
+    <row r="26" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="70" t="s">
         <v>278</v>
       </c>
-      <c r="E23" s="33" t="s">
+      <c r="E26" s="33" t="s">
         <v>273</v>
       </c>
-      <c r="F23" s="74" t="s">
+      <c r="F26" s="74" t="s">
         <v>274</v>
       </c>
-      <c r="I23" s="78" t="s">
+      <c r="I26" s="78" t="s">
         <v>275</v>
       </c>
-      <c r="J23" s="79" t="s">
+      <c r="J26" s="79" t="s">
         <v>276</v>
       </c>
-      <c r="K23" s="10" t="s">
+      <c r="K26" s="10" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="24" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="71" t="s">
+    <row r="27" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="71" t="s">
         <v>283</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="E27" s="33" t="s">
         <v>279</v>
       </c>
-      <c r="F24" s="75" t="s">
+      <c r="F27" s="75" t="s">
         <v>280</v>
       </c>
-      <c r="I24" s="78" t="s">
+      <c r="I27" s="78" t="s">
         <v>281</v>
       </c>
-      <c r="J24" s="9" t="s">
+      <c r="J27" s="9" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E25" s="67" t="s">
+    <row r="28" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="67" t="s">
         <v>284</v>
       </c>
-      <c r="F25" s="68"/>
-      <c r="I25" s="80" t="s">
+      <c r="F28" s="68"/>
+      <c r="I28" s="80" t="s">
         <v>285</v>
       </c>
-      <c r="J25" s="9" t="s">
+      <c r="J28" s="9" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="26" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J26" s="71" t="s">
+    <row r="29" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J29" s="71" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="27" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="113" t="s">
+    <row r="30" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="113" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="29" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="111" t="s">
+    <row r="32" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="111" t="s">
         <v>434</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34" s="187"/>
-      <c r="D34" s="187"/>
+      <c r="C34" s="160"/>
+      <c r="D34" s="160"/>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C35"/>
@@ -5262,49 +5278,50 @@
       <c r="D37"/>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C38" s="187"/>
-      <c r="D38" s="187"/>
+      <c r="C38" s="160"/>
+      <c r="D38" s="160"/>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C39" s="187"/>
-      <c r="D39" s="187"/>
+      <c r="C39" s="160"/>
+      <c r="D39" s="160"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="35">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="F19:G19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -5373,7 +5390,7 @@
       <c r="C7" s="116" t="s">
         <v>297</v>
       </c>
-      <c r="D7" s="191" t="s">
+      <c r="D7" s="192" t="s">
         <v>455</v>
       </c>
     </row>
@@ -5384,7 +5401,7 @@
       <c r="C8" s="116" t="s">
         <v>299</v>
       </c>
-      <c r="D8" s="192"/>
+      <c r="D8" s="193"/>
     </row>
     <row r="9" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="108" t="s">
@@ -5393,7 +5410,7 @@
       <c r="C9" s="116" t="s">
         <v>301</v>
       </c>
-      <c r="D9" s="192"/>
+      <c r="D9" s="193"/>
     </row>
     <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="108" t="s">
@@ -5402,7 +5419,7 @@
       <c r="C10" s="116" t="s">
         <v>302</v>
       </c>
-      <c r="D10" s="192"/>
+      <c r="D10" s="193"/>
     </row>
     <row r="11" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="108" t="s">
@@ -5411,7 +5428,7 @@
       <c r="C11" s="116" t="s">
         <v>304</v>
       </c>
-      <c r="D11" s="192"/>
+      <c r="D11" s="193"/>
     </row>
     <row r="12" spans="2:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B12" s="108" t="s">
@@ -5420,7 +5437,7 @@
       <c r="C12" s="116" t="s">
         <v>306</v>
       </c>
-      <c r="D12" s="192"/>
+      <c r="D12" s="193"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="108" t="s">
@@ -5429,7 +5446,7 @@
       <c r="C13" s="116" t="s">
         <v>308</v>
       </c>
-      <c r="D13" s="192"/>
+      <c r="D13" s="193"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="108" t="s">
@@ -5438,7 +5455,7 @@
       <c r="C14" s="116" t="s">
         <v>310</v>
       </c>
-      <c r="D14" s="192"/>
+      <c r="D14" s="193"/>
     </row>
     <row r="15" spans="2:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="109" t="s">
@@ -5447,7 +5464,7 @@
       <c r="C15" s="114" t="s">
         <v>312</v>
       </c>
-      <c r="D15" s="193"/>
+      <c r="D15" s="194"/>
     </row>
     <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5499,7 +5516,7 @@
       <c r="C24" s="116" t="s">
         <v>323</v>
       </c>
-      <c r="D24" s="191" t="s">
+      <c r="D24" s="192" t="s">
         <v>324</v>
       </c>
     </row>
@@ -5510,7 +5527,7 @@
       <c r="C25" s="116" t="s">
         <v>326</v>
       </c>
-      <c r="D25" s="192"/>
+      <c r="D25" s="193"/>
     </row>
     <row r="26" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="108" t="s">
@@ -5519,7 +5536,7 @@
       <c r="C26" s="116" t="s">
         <v>328</v>
       </c>
-      <c r="D26" s="195"/>
+      <c r="D26" s="196"/>
     </row>
     <row r="27" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="108" t="s">
@@ -5617,7 +5634,7 @@
       <c r="C37" s="149" t="s">
         <v>349</v>
       </c>
-      <c r="D37" s="194" t="s">
+      <c r="D37" s="195" t="s">
         <v>350</v>
       </c>
     </row>
@@ -5628,7 +5645,7 @@
       <c r="C38" s="116" t="s">
         <v>352</v>
       </c>
-      <c r="D38" s="195"/>
+      <c r="D38" s="196"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="108"/>
@@ -5697,7 +5714,7 @@
         <v>354</v>
       </c>
       <c r="C51" s="149"/>
-      <c r="D51" s="194" t="s">
+      <c r="D51" s="195" t="s">
         <v>355</v>
       </c>
     </row>
@@ -5706,14 +5723,14 @@
         <v>356</v>
       </c>
       <c r="C52" s="116"/>
-      <c r="D52" s="192"/>
+      <c r="D52" s="193"/>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="108" t="s">
         <v>357</v>
       </c>
       <c r="C53" s="116"/>
-      <c r="D53" s="195"/>
+      <c r="D53" s="196"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="108"/>
@@ -5796,7 +5813,7 @@
       <c r="C66" s="116" t="s">
         <v>467</v>
       </c>
-      <c r="D66" s="194" t="s">
+      <c r="D66" s="195" t="s">
         <v>465</v>
       </c>
     </row>
@@ -5807,7 +5824,7 @@
       <c r="C67" s="116" t="s">
         <v>461</v>
       </c>
-      <c r="D67" s="192"/>
+      <c r="D67" s="193"/>
     </row>
     <row r="68" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="108" t="s">
@@ -5816,7 +5833,7 @@
       <c r="C68" s="116" t="s">
         <v>462</v>
       </c>
-      <c r="D68" s="192"/>
+      <c r="D68" s="193"/>
     </row>
     <row r="69" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B69" s="108" t="s">
@@ -5825,7 +5842,7 @@
       <c r="C69" s="116" t="s">
         <v>463</v>
       </c>
-      <c r="D69" s="192"/>
+      <c r="D69" s="193"/>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="108" t="s">
@@ -5834,7 +5851,7 @@
       <c r="C70" s="116" t="s">
         <v>464</v>
       </c>
-      <c r="D70" s="195"/>
+      <c r="D70" s="196"/>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="108"/>
@@ -5865,19 +5882,19 @@
     <row r="80" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B80" s="95"/>
       <c r="C80" s="95"/>
-      <c r="D80" s="196"/>
+      <c r="D80" s="197"/>
       <c r="E80" s="95"/>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" s="95"/>
       <c r="C81" s="95"/>
-      <c r="D81" s="196"/>
+      <c r="D81" s="197"/>
       <c r="E81" s="95"/>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="95"/>
       <c r="C82" s="95"/>
-      <c r="D82" s="196"/>
+      <c r="D82" s="197"/>
       <c r="E82" s="95"/>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added more Zaun Creatures
Changes made in extracted 'set' file. Need to be compressed into .mse-set file.
Minor updates to DesignDoc (expanding on faction abilities)
</commit_message>
<xml_diff>
--- a/DesignDoc.xlsx
+++ b/DesignDoc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4815" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4815"/>
   </bookViews>
   <sheets>
     <sheet name="Factions" sheetId="6" r:id="rId1"/>
@@ -1264,9 +1264,6 @@
     <t>Keywords and Abilites</t>
   </si>
   <si>
-    <t>Spawn</t>
-  </si>
-  <si>
     <t>Swarm</t>
   </si>
   <si>
@@ -1304,11 +1301,6 @@
   <si>
     <t>Noxus just want to attack and destroy anything that stands in its way. They have no patience for the weak. They cripple their enemies and thrive on the smell of their blood.
 -1/-1 counters to cripple their enemies. Executions and Blood Thirst to reward aggression.</t>
-  </si>
-  <si>
-    <t>Greiveous Wounds
-Execute
-Blood Thirst</t>
   </si>
   <si>
     <t>Ionians want a peaceful existence away from the wars of the mainland. When confronted with direct aggression, they patiently meet it with de-escalation. 
@@ -1413,9 +1405,6 @@
   </si>
   <si>
     <t>Evolution</t>
-  </si>
-  <si>
-    <t>Adapt / Evolve</t>
   </si>
   <si>
     <t>The scientists of Zaun are always on the cutting edge of new discoveries. They tirelessly concoct potions and develop new technologies
@@ -1569,6 +1558,18 @@
       </rPr>
       <t xml:space="preserve"> These are just ideas for names.</t>
     </r>
+  </si>
+  <si>
+    <t>-1/-1 Counters
+Greiveous Wounds</t>
+  </si>
+  <si>
+    <t>Adapt / Evolve
+Tribal</t>
+  </si>
+  <si>
+    <t>Spawn
+Tribal</t>
   </si>
 </sst>
 </file>
@@ -3126,6 +3127,93 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3136,90 +3224,6 @@
     <xf numFmtId="0" fontId="1" fillId="33" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3237,9 +3241,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3534,8 +3535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3579,13 +3580,13 @@
         <v>394</v>
       </c>
       <c r="D3" s="98" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E3" s="98" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F3" s="99" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3600,10 +3601,10 @@
         <v>384</v>
       </c>
       <c r="E4" s="96" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="F4" s="100" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3615,13 +3616,13 @@
         <v>393</v>
       </c>
       <c r="D5" s="96" t="s">
-        <v>405</v>
-      </c>
-      <c r="E5" s="96" t="s">
-        <v>414</v>
+        <v>404</v>
+      </c>
+      <c r="E5" s="97" t="s">
+        <v>485</v>
       </c>
       <c r="F5" s="101" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3639,7 +3640,7 @@
         <v>392</v>
       </c>
       <c r="F6" s="100" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3657,7 +3658,7 @@
         <v>398</v>
       </c>
       <c r="F7" s="100" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3666,16 +3667,16 @@
         <v>371</v>
       </c>
       <c r="C8" s="116" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D8" s="96" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E8" s="96" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F8" s="100" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3687,13 +3688,13 @@
         <v>391</v>
       </c>
       <c r="D9" s="96" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E9" s="96" t="s">
-        <v>401</v>
+        <v>487</v>
       </c>
       <c r="F9" s="100" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3702,7 +3703,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="116" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D10" s="96" t="s">
         <v>386</v>
@@ -3711,7 +3712,7 @@
         <v>390</v>
       </c>
       <c r="F10" s="101" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3720,16 +3721,16 @@
         <v>20</v>
       </c>
       <c r="C11" s="116" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D11" s="96" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E11" s="96" t="s">
         <v>389</v>
       </c>
       <c r="F11" s="100" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3738,16 +3739,16 @@
         <v>17</v>
       </c>
       <c r="C12" s="116" t="s">
+        <v>406</v>
+      </c>
+      <c r="D12" s="96" t="s">
         <v>407</v>
       </c>
-      <c r="D12" s="96" t="s">
-        <v>408</v>
-      </c>
       <c r="E12" s="96" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="F12" s="100" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3755,16 +3756,16 @@
         <v>258</v>
       </c>
       <c r="C13" s="114" t="s">
+        <v>443</v>
+      </c>
+      <c r="D13" s="102" t="s">
+        <v>436</v>
+      </c>
+      <c r="E13" s="102" t="s">
+        <v>486</v>
+      </c>
+      <c r="F13" s="103" t="s">
         <v>445</v>
-      </c>
-      <c r="D13" s="102" t="s">
-        <v>438</v>
-      </c>
-      <c r="E13" s="102" t="s">
-        <v>446</v>
-      </c>
-      <c r="F13" s="103" t="s">
-        <v>448</v>
       </c>
     </row>
   </sheetData>
@@ -3792,7 +3793,7 @@
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="90" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C2" s="91" t="s">
         <v>0</v>
@@ -3806,36 +3807,36 @@
     </row>
     <row r="3" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="107" t="s">
+        <v>419</v>
+      </c>
+      <c r="C3" s="104" t="s">
+        <v>420</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>421</v>
       </c>
-      <c r="C3" s="104" t="s">
-        <v>422</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>423</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="109" t="s">
+        <v>422</v>
+      </c>
+      <c r="C4" s="106" t="s">
+        <v>423</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>424</v>
       </c>
-      <c r="C4" s="106" t="s">
+      <c r="E4" s="7" t="s">
         <v>425</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>426</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="90" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C6" s="91" t="s">
         <v>0</v>
@@ -3876,7 +3877,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="105" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>376</v>
@@ -3896,7 +3897,7 @@
         <v>375</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -3947,16 +3948,16 @@
     </row>
     <row r="15" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B15" s="108" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C15" s="105" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>440</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="45" x14ac:dyDescent="0.25">
@@ -3973,10 +3974,10 @@
     </row>
     <row r="17" spans="1:5" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="109" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C17" s="106" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>372</v>
@@ -3989,14 +3990,14 @@
       <c r="A19" s="156"/>
       <c r="B19" s="156"/>
       <c r="C19" s="157" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="D19" s="156"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="156"/>
       <c r="B20" s="90" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C20" s="91" t="s">
         <v>0</v>
@@ -4008,25 +4009,25 @@
     <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="156"/>
       <c r="B21" s="107" t="s">
+        <v>474</v>
+      </c>
+      <c r="C21" s="104" t="s">
         <v>477</v>
       </c>
-      <c r="C21" s="104" t="s">
-        <v>480</v>
-      </c>
       <c r="D21" s="3" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="156"/>
       <c r="B22" s="109" t="s">
+        <v>475</v>
+      </c>
+      <c r="C22" s="106" t="s">
+        <v>476</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>478</v>
-      </c>
-      <c r="C22" s="106" t="s">
-        <v>479</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>481</v>
       </c>
     </row>
   </sheetData>
@@ -4264,7 +4265,7 @@
         <v>9</v>
       </c>
       <c r="E13" s="27" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F13" s="28" t="s">
         <v>14</v>
@@ -4759,7 +4760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
@@ -4771,10 +4772,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="198" t="s">
-        <v>487</v>
-      </c>
-      <c r="C2" s="198"/>
+      <c r="B2" s="160" t="s">
+        <v>484</v>
+      </c>
+      <c r="C2" s="160"/>
     </row>
     <row r="3" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4785,26 +4786,26 @@
       <c r="F4"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="182" t="s">
+      <c r="B5" s="165" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="183"/>
-      <c r="D5" s="184" t="s">
+      <c r="C5" s="166"/>
+      <c r="D5" s="167" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="185"/>
-      <c r="F5" s="186" t="s">
+      <c r="E5" s="168"/>
+      <c r="F5" s="169" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="187"/>
-      <c r="H5" s="188" t="s">
+      <c r="G5" s="170"/>
+      <c r="H5" s="171" t="s">
         <v>382</v>
       </c>
-      <c r="I5" s="189"/>
-      <c r="J5" s="190" t="s">
+      <c r="I5" s="172"/>
+      <c r="J5" s="173" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="191"/>
+      <c r="K5" s="174"/>
     </row>
     <row r="6" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="39" t="s">
@@ -4849,7 +4850,7 @@
         <v>210</v>
       </c>
       <c r="E7" s="49" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="F7" s="62" t="s">
         <v>211</v>
@@ -4890,7 +4891,7 @@
         <v>222</v>
       </c>
       <c r="H8" s="33" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="I8" s="34" t="s">
         <v>223</v>
@@ -4903,48 +4904,48 @@
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="164" t="s">
+      <c r="B9" s="161" t="s">
         <v>226</v>
       </c>
-      <c r="C9" s="166"/>
-      <c r="D9" s="164" t="s">
-        <v>472</v>
-      </c>
-      <c r="E9" s="165"/>
-      <c r="F9" s="167" t="s">
+      <c r="C9" s="162"/>
+      <c r="D9" s="161" t="s">
+        <v>469</v>
+      </c>
+      <c r="E9" s="163"/>
+      <c r="F9" s="164" t="s">
         <v>227</v>
       </c>
-      <c r="G9" s="166"/>
-      <c r="H9" s="164" t="s">
+      <c r="G9" s="162"/>
+      <c r="H9" s="161" t="s">
         <v>228</v>
       </c>
-      <c r="I9" s="165"/>
-      <c r="J9" s="167" t="s">
+      <c r="I9" s="163"/>
+      <c r="J9" s="164" t="s">
         <v>229</v>
       </c>
-      <c r="K9" s="165"/>
+      <c r="K9" s="163"/>
     </row>
     <row r="10" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="168" t="s">
+      <c r="B10" s="185" t="s">
         <v>230</v>
       </c>
-      <c r="C10" s="170"/>
-      <c r="D10" s="168" t="s">
+      <c r="C10" s="186"/>
+      <c r="D10" s="185" t="s">
         <v>231</v>
       </c>
-      <c r="E10" s="169"/>
-      <c r="F10" s="171" t="s">
-        <v>474</v>
-      </c>
-      <c r="G10" s="170"/>
-      <c r="H10" s="168" t="s">
-        <v>468</v>
-      </c>
-      <c r="I10" s="169"/>
-      <c r="J10" s="171" t="s">
+      <c r="E10" s="187"/>
+      <c r="F10" s="188" t="s">
+        <v>471</v>
+      </c>
+      <c r="G10" s="186"/>
+      <c r="H10" s="185" t="s">
+        <v>465</v>
+      </c>
+      <c r="I10" s="187"/>
+      <c r="J10" s="188" t="s">
         <v>232</v>
       </c>
-      <c r="K10" s="169"/>
+      <c r="K10" s="187"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12"/>
@@ -4961,26 +4962,26 @@
       <c r="F13"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="172" t="s">
+      <c r="B14" s="175" t="s">
         <v>371</v>
       </c>
-      <c r="C14" s="173"/>
-      <c r="D14" s="174" t="s">
+      <c r="C14" s="176"/>
+      <c r="D14" s="177" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="175"/>
-      <c r="F14" s="176" t="s">
+      <c r="E14" s="178"/>
+      <c r="F14" s="179" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="177"/>
-      <c r="H14" s="178" t="s">
+      <c r="G14" s="180"/>
+      <c r="H14" s="181" t="s">
         <v>20</v>
       </c>
-      <c r="I14" s="179"/>
-      <c r="J14" s="180" t="s">
+      <c r="I14" s="182"/>
+      <c r="J14" s="183" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="181"/>
+      <c r="K14" s="184"/>
     </row>
     <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="51" t="s">
@@ -5019,7 +5020,7 @@
         <v>388</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="D16" s="66" t="s">
         <v>236</v>
@@ -5049,7 +5050,7 @@
         <v>249</v>
       </c>
       <c r="C17" s="36" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="D17" s="64" t="s">
         <v>243</v>
@@ -5075,48 +5076,48 @@
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="164" t="s">
-        <v>484</v>
-      </c>
-      <c r="C18" s="165"/>
-      <c r="D18" s="167" t="s">
+      <c r="B18" s="161" t="s">
+        <v>481</v>
+      </c>
+      <c r="C18" s="163"/>
+      <c r="D18" s="164" t="s">
         <v>248</v>
       </c>
-      <c r="E18" s="165"/>
-      <c r="F18" s="167" t="s">
+      <c r="E18" s="163"/>
+      <c r="F18" s="164" t="s">
         <v>250</v>
       </c>
-      <c r="G18" s="166"/>
-      <c r="H18" s="164" t="s">
+      <c r="G18" s="162"/>
+      <c r="H18" s="161" t="s">
         <v>247</v>
       </c>
-      <c r="I18" s="166"/>
-      <c r="J18" s="164" t="s">
-        <v>434</v>
-      </c>
-      <c r="K18" s="165"/>
+      <c r="I18" s="162"/>
+      <c r="J18" s="161" t="s">
+        <v>432</v>
+      </c>
+      <c r="K18" s="163"/>
     </row>
     <row r="19" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="168" t="s">
+      <c r="B19" s="185" t="s">
         <v>253</v>
       </c>
-      <c r="C19" s="169"/>
-      <c r="D19" s="171" t="s">
+      <c r="C19" s="187"/>
+      <c r="D19" s="188" t="s">
         <v>252</v>
       </c>
-      <c r="E19" s="169"/>
-      <c r="F19" s="171" t="s">
+      <c r="E19" s="187"/>
+      <c r="F19" s="188" t="s">
         <v>254</v>
       </c>
-      <c r="G19" s="170"/>
-      <c r="H19" s="168" t="s">
+      <c r="G19" s="186"/>
+      <c r="H19" s="185" t="s">
         <v>251</v>
       </c>
-      <c r="I19" s="170"/>
-      <c r="J19" s="168" t="s">
-        <v>471</v>
-      </c>
-      <c r="K19" s="169"/>
+      <c r="I19" s="186"/>
+      <c r="J19" s="185" t="s">
+        <v>468</v>
+      </c>
+      <c r="K19" s="187"/>
     </row>
     <row r="21" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
@@ -5130,11 +5131,11 @@
         <v>256</v>
       </c>
       <c r="G22" s="8"/>
-      <c r="I22" s="161" t="s">
+      <c r="I22" s="190" t="s">
         <v>257</v>
       </c>
-      <c r="J22" s="162"/>
-      <c r="K22" s="163"/>
+      <c r="J22" s="191"/>
+      <c r="K22" s="192"/>
     </row>
     <row r="23" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="81" t="s">
@@ -5158,7 +5159,7 @@
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="E24" s="31" t="s">
         <v>262</v>
@@ -5253,17 +5254,17 @@
     <row r="30" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="113" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="32" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="111" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34" s="160"/>
-      <c r="D34" s="160"/>
+      <c r="C34" s="189"/>
+      <c r="D34" s="189"/>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C35"/>
@@ -5278,36 +5279,15 @@
       <c r="D37"/>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C38" s="160"/>
-      <c r="D38" s="160"/>
+      <c r="C38" s="189"/>
+      <c r="D38" s="189"/>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C39" s="160"/>
-      <c r="D39" s="160"/>
+      <c r="C39" s="189"/>
+      <c r="D39" s="189"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="C38:D38"/>
@@ -5322,6 +5302,27 @@
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="J19:K19"/>
     <mergeCell ref="F19:G19"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -5390,8 +5391,8 @@
       <c r="C7" s="116" t="s">
         <v>297</v>
       </c>
-      <c r="D7" s="192" t="s">
-        <v>455</v>
+      <c r="D7" s="193" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -5401,7 +5402,7 @@
       <c r="C8" s="116" t="s">
         <v>299</v>
       </c>
-      <c r="D8" s="193"/>
+      <c r="D8" s="194"/>
     </row>
     <row r="9" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="108" t="s">
@@ -5410,16 +5411,16 @@
       <c r="C9" s="116" t="s">
         <v>301</v>
       </c>
-      <c r="D9" s="193"/>
+      <c r="D9" s="194"/>
     </row>
     <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="108" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="C10" s="116" t="s">
         <v>302</v>
       </c>
-      <c r="D10" s="193"/>
+      <c r="D10" s="194"/>
     </row>
     <row r="11" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="108" t="s">
@@ -5428,7 +5429,7 @@
       <c r="C11" s="116" t="s">
         <v>304</v>
       </c>
-      <c r="D11" s="193"/>
+      <c r="D11" s="194"/>
     </row>
     <row r="12" spans="2:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B12" s="108" t="s">
@@ -5437,7 +5438,7 @@
       <c r="C12" s="116" t="s">
         <v>306</v>
       </c>
-      <c r="D12" s="193"/>
+      <c r="D12" s="194"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="108" t="s">
@@ -5446,7 +5447,7 @@
       <c r="C13" s="116" t="s">
         <v>308</v>
       </c>
-      <c r="D13" s="193"/>
+      <c r="D13" s="194"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="108" t="s">
@@ -5455,7 +5456,7 @@
       <c r="C14" s="116" t="s">
         <v>310</v>
       </c>
-      <c r="D14" s="193"/>
+      <c r="D14" s="194"/>
     </row>
     <row r="15" spans="2:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="109" t="s">
@@ -5464,7 +5465,7 @@
       <c r="C15" s="114" t="s">
         <v>312</v>
       </c>
-      <c r="D15" s="194"/>
+      <c r="D15" s="195"/>
     </row>
     <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5516,7 +5517,7 @@
       <c r="C24" s="116" t="s">
         <v>323</v>
       </c>
-      <c r="D24" s="192" t="s">
+      <c r="D24" s="193" t="s">
         <v>324</v>
       </c>
     </row>
@@ -5527,7 +5528,7 @@
       <c r="C25" s="116" t="s">
         <v>326</v>
       </c>
-      <c r="D25" s="193"/>
+      <c r="D25" s="194"/>
     </row>
     <row r="26" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="108" t="s">
@@ -5536,7 +5537,7 @@
       <c r="C26" s="116" t="s">
         <v>328</v>
       </c>
-      <c r="D26" s="196"/>
+      <c r="D26" s="197"/>
     </row>
     <row r="27" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="108" t="s">
@@ -5634,7 +5635,7 @@
       <c r="C37" s="149" t="s">
         <v>349</v>
       </c>
-      <c r="D37" s="195" t="s">
+      <c r="D37" s="196" t="s">
         <v>350</v>
       </c>
     </row>
@@ -5645,7 +5646,7 @@
       <c r="C38" s="116" t="s">
         <v>352</v>
       </c>
-      <c r="D38" s="196"/>
+      <c r="D38" s="197"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="108"/>
@@ -5714,7 +5715,7 @@
         <v>354</v>
       </c>
       <c r="C51" s="149"/>
-      <c r="D51" s="195" t="s">
+      <c r="D51" s="196" t="s">
         <v>355</v>
       </c>
     </row>
@@ -5723,14 +5724,14 @@
         <v>356</v>
       </c>
       <c r="C52" s="116"/>
-      <c r="D52" s="193"/>
+      <c r="D52" s="194"/>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="108" t="s">
         <v>357</v>
       </c>
       <c r="C53" s="116"/>
-      <c r="D53" s="196"/>
+      <c r="D53" s="197"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="108"/>
@@ -5797,7 +5798,7 @@
     <row r="64" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="65" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="154" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C65" s="155" t="s">
         <v>289</v>
@@ -5808,50 +5809,50 @@
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="108" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="C66" s="116" t="s">
-        <v>467</v>
-      </c>
-      <c r="D66" s="195" t="s">
-        <v>465</v>
+        <v>464</v>
+      </c>
+      <c r="D66" s="196" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="67" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B67" s="108" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="C67" s="116" t="s">
-        <v>461</v>
-      </c>
-      <c r="D67" s="193"/>
+        <v>458</v>
+      </c>
+      <c r="D67" s="194"/>
     </row>
     <row r="68" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="108" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C68" s="116" t="s">
-        <v>462</v>
-      </c>
-      <c r="D68" s="193"/>
+        <v>459</v>
+      </c>
+      <c r="D68" s="194"/>
     </row>
     <row r="69" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B69" s="108" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C69" s="116" t="s">
-        <v>463</v>
-      </c>
-      <c r="D69" s="193"/>
+        <v>460</v>
+      </c>
+      <c r="D69" s="194"/>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="108" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C70" s="116" t="s">
-        <v>464</v>
-      </c>
-      <c r="D70" s="196"/>
+        <v>461</v>
+      </c>
+      <c r="D70" s="197"/>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="108"/>
@@ -5882,19 +5883,19 @@
     <row r="80" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B80" s="95"/>
       <c r="C80" s="95"/>
-      <c r="D80" s="197"/>
+      <c r="D80" s="198"/>
       <c r="E80" s="95"/>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" s="95"/>
       <c r="C81" s="95"/>
-      <c r="D81" s="197"/>
+      <c r="D81" s="198"/>
       <c r="E81" s="95"/>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="95"/>
       <c r="C82" s="95"/>
-      <c r="D82" s="197"/>
+      <c r="D82" s="198"/>
       <c r="E82" s="95"/>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
@@ -6086,7 +6087,7 @@
         <v>9</v>
       </c>
       <c r="E13" s="137" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F13" s="138" t="s">
         <v>14</v>
@@ -6097,13 +6098,13 @@
         <v>368</v>
       </c>
       <c r="C14" s="112" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="D14" s="112" t="s">
         <v>365</v>
       </c>
       <c r="E14" s="112" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="F14" s="49" t="s">
         <v>364</v>
@@ -6167,16 +6168,16 @@
         <v>366</v>
       </c>
       <c r="C23" s="112" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="D23" s="112" t="s">
         <v>28</v>
       </c>
       <c r="E23" s="112" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="F23" s="49" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added card type distribution to DesignDoc
</commit_message>
<xml_diff>
--- a/DesignDoc.xlsx
+++ b/DesignDoc.xlsx
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4815"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4815" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Factions" sheetId="6" r:id="rId1"/>
     <sheet name="Types and Keywords" sheetId="1" r:id="rId2"/>
-    <sheet name="Champions" sheetId="2" r:id="rId3"/>
-    <sheet name="Non-Champions" sheetId="3" r:id="rId4"/>
-    <sheet name="Artifacts and Enchantments" sheetId="4" r:id="rId5"/>
-    <sheet name="Instants and Sorceries" sheetId="5" r:id="rId6"/>
+    <sheet name="Type and Color Distributions" sheetId="7" r:id="rId3"/>
+    <sheet name="Champions" sheetId="2" r:id="rId4"/>
+    <sheet name="Non-Champions" sheetId="3" r:id="rId5"/>
+    <sheet name="Artifacts and Enchantments" sheetId="4" r:id="rId6"/>
+    <sheet name="Instants and Sorceries" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="523">
   <si>
     <t>Description</t>
   </si>
@@ -1571,6 +1572,111 @@
     <t>Spawn
 Tribal</t>
   </si>
+  <si>
+    <t>Creatures</t>
+  </si>
+  <si>
+    <t>Permanents</t>
+  </si>
+  <si>
+    <t>Spells</t>
+  </si>
+  <si>
+    <t>Artifacts</t>
+  </si>
+  <si>
+    <t>Enchantments</t>
+  </si>
+  <si>
+    <t>Auras</t>
+  </si>
+  <si>
+    <t>Runes</t>
+  </si>
+  <si>
+    <t>Planeswalkers</t>
+  </si>
+  <si>
+    <t>Instants</t>
+  </si>
+  <si>
+    <t>Sorceries</t>
+  </si>
+  <si>
+    <t>Card Type</t>
+  </si>
+  <si>
+    <t>Land</t>
+  </si>
+  <si>
+    <t>Plains</t>
+  </si>
+  <si>
+    <t>Island</t>
+  </si>
+  <si>
+    <t>Swamp</t>
+  </si>
+  <si>
+    <t>Mountain</t>
+  </si>
+  <si>
+    <t>Forest</t>
+  </si>
+  <si>
+    <t>Basic Land</t>
+  </si>
+  <si>
+    <t>Legendary Land</t>
+  </si>
+  <si>
+    <t>Capital of Demacia</t>
+  </si>
+  <si>
+    <t>Howling Abyss</t>
+  </si>
+  <si>
+    <t>Immortal Bastion</t>
+  </si>
+  <si>
+    <t>Kumunga Jungle</t>
+  </si>
+  <si>
+    <t>Mount Targon</t>
+  </si>
+  <si>
+    <t>Placidium of Navori</t>
+  </si>
+  <si>
+    <t>Perished Lands</t>
+  </si>
+  <si>
+    <t>Port of Piltover</t>
+  </si>
+  <si>
+    <t>Sewers of Zaun</t>
+  </si>
+  <si>
+    <t>City of the Sun Disc</t>
+  </si>
+  <si>
+    <t>Portal to the Void</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Tap Land</t>
+  </si>
+  <si>
+    <t>Non-Champions</t>
+  </si>
+  <si>
+    <t>Non-Auras</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
 </sst>
 </file>
 
@@ -1593,7 +1699,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1895,6 +2001,12 @@
         </stop>
       </gradientFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="59">
     <border>
@@ -2652,7 +2764,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="199">
+  <cellXfs count="211">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3121,99 +3233,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3222,6 +3283,93 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3535,8 +3683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3777,8 +3925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4038,10 +4186,813 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" style="167" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="158" customWidth="1"/>
+    <col min="3" max="18" width="20.140625" style="158" customWidth="1"/>
+    <col min="19" max="16384" width="16.85546875" style="158"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="168" t="s">
+        <v>498</v>
+      </c>
+      <c r="B2" s="163" t="s">
+        <v>518</v>
+      </c>
+      <c r="C2" s="128" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="129" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="164" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="131" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="165" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="166" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="135" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="136" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="137" t="s">
+        <v>382</v>
+      </c>
+      <c r="L2" s="159" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="160" t="s">
+        <v>371</v>
+      </c>
+      <c r="N2" s="140" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="141" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="142" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="161" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" s="162" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="168"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="168" t="s">
+        <v>499</v>
+      </c>
+      <c r="B4" s="158">
+        <f>SUM(B7,B6,B8)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="169"/>
+      <c r="C5" s="163"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="169" t="s">
+        <v>505</v>
+      </c>
+      <c r="B6" s="158">
+        <v>5</v>
+      </c>
+      <c r="C6" s="158" t="s">
+        <v>500</v>
+      </c>
+      <c r="D6" s="158" t="s">
+        <v>501</v>
+      </c>
+      <c r="E6" s="158" t="s">
+        <v>502</v>
+      </c>
+      <c r="F6" s="158" t="s">
+        <v>503</v>
+      </c>
+      <c r="G6" s="158" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="169" t="s">
+        <v>519</v>
+      </c>
+      <c r="B7" s="158">
+        <v>10</v>
+      </c>
+      <c r="H7" s="158" t="s">
+        <v>507</v>
+      </c>
+      <c r="I7" s="158" t="s">
+        <v>508</v>
+      </c>
+      <c r="J7" s="158" t="s">
+        <v>509</v>
+      </c>
+      <c r="K7" s="158" t="s">
+        <v>510</v>
+      </c>
+      <c r="L7" s="158" t="s">
+        <v>512</v>
+      </c>
+      <c r="M7" s="158" t="s">
+        <v>511</v>
+      </c>
+      <c r="N7" s="158" t="s">
+        <v>513</v>
+      </c>
+      <c r="O7" s="158" t="s">
+        <v>515</v>
+      </c>
+      <c r="P7" s="158" t="s">
+        <v>514</v>
+      </c>
+      <c r="Q7" s="158" t="s">
+        <v>516</v>
+      </c>
+      <c r="R7" s="158" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="169" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="168"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="168" t="s">
+        <v>489</v>
+      </c>
+      <c r="B10" s="158">
+        <f>SUM(B12,B14,B16,B19,B23,B25,-B23, -B23)</f>
+        <v>428</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="168"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="169" t="s">
+        <v>488</v>
+      </c>
+      <c r="B12" s="158">
+        <f>SUM(B13,B14)</f>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="167" t="s">
+        <v>520</v>
+      </c>
+      <c r="B13" s="158">
+        <f>SUM(C13:R13)</f>
+        <v>120</v>
+      </c>
+      <c r="C13" s="158">
+        <v>10</v>
+      </c>
+      <c r="D13" s="158">
+        <v>10</v>
+      </c>
+      <c r="E13" s="158">
+        <v>10</v>
+      </c>
+      <c r="F13" s="158">
+        <v>10</v>
+      </c>
+      <c r="G13" s="158">
+        <v>10</v>
+      </c>
+      <c r="H13" s="158">
+        <v>6</v>
+      </c>
+      <c r="I13" s="158">
+        <v>6</v>
+      </c>
+      <c r="J13" s="158">
+        <v>6</v>
+      </c>
+      <c r="K13" s="158">
+        <v>6</v>
+      </c>
+      <c r="L13" s="158">
+        <v>6</v>
+      </c>
+      <c r="M13" s="158">
+        <v>6</v>
+      </c>
+      <c r="N13" s="158">
+        <v>6</v>
+      </c>
+      <c r="O13" s="158">
+        <v>6</v>
+      </c>
+      <c r="P13" s="158">
+        <v>6</v>
+      </c>
+      <c r="Q13" s="158">
+        <v>6</v>
+      </c>
+      <c r="R13" s="158">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="169" t="s">
+        <v>188</v>
+      </c>
+      <c r="B14" s="158">
+        <f>SUM(C14:R14)</f>
+        <v>113</v>
+      </c>
+      <c r="C14" s="158">
+        <v>9</v>
+      </c>
+      <c r="D14" s="158">
+        <v>9</v>
+      </c>
+      <c r="E14" s="158">
+        <v>9</v>
+      </c>
+      <c r="F14" s="158">
+        <v>9</v>
+      </c>
+      <c r="G14" s="158">
+        <v>9</v>
+      </c>
+      <c r="H14" s="158">
+        <v>6</v>
+      </c>
+      <c r="I14" s="158">
+        <v>6</v>
+      </c>
+      <c r="J14" s="158">
+        <v>6</v>
+      </c>
+      <c r="K14" s="158">
+        <v>6</v>
+      </c>
+      <c r="L14" s="158">
+        <v>6</v>
+      </c>
+      <c r="M14" s="158">
+        <v>6</v>
+      </c>
+      <c r="N14" s="158">
+        <v>6</v>
+      </c>
+      <c r="O14" s="158">
+        <v>6</v>
+      </c>
+      <c r="P14" s="158">
+        <v>6</v>
+      </c>
+      <c r="Q14" s="158">
+        <v>6</v>
+      </c>
+      <c r="R14" s="158">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="169"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="169" t="s">
+        <v>491</v>
+      </c>
+      <c r="B16" s="158">
+        <f>SUM(C16:R16,B17, B23)</f>
+        <v>40</v>
+      </c>
+      <c r="C16" s="158">
+        <v>1</v>
+      </c>
+      <c r="D16" s="158">
+        <v>1</v>
+      </c>
+      <c r="E16" s="158">
+        <v>1</v>
+      </c>
+      <c r="F16" s="158">
+        <v>1</v>
+      </c>
+      <c r="G16" s="158">
+        <v>1</v>
+      </c>
+      <c r="H16" s="158">
+        <v>0</v>
+      </c>
+      <c r="I16" s="158">
+        <v>0</v>
+      </c>
+      <c r="J16" s="158">
+        <v>0</v>
+      </c>
+      <c r="K16" s="158">
+        <v>0</v>
+      </c>
+      <c r="L16" s="158">
+        <v>0</v>
+      </c>
+      <c r="M16" s="158">
+        <v>0</v>
+      </c>
+      <c r="N16" s="158">
+        <v>0</v>
+      </c>
+      <c r="O16" s="158">
+        <v>0</v>
+      </c>
+      <c r="P16" s="158">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="158">
+        <v>0</v>
+      </c>
+      <c r="R16" s="158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="169" t="s">
+        <v>313</v>
+      </c>
+      <c r="B17" s="158">
+        <f>SUM(C17:R17)</f>
+        <v>10</v>
+      </c>
+      <c r="C17" s="158">
+        <v>0</v>
+      </c>
+      <c r="D17" s="158">
+        <v>0</v>
+      </c>
+      <c r="E17" s="158">
+        <v>0</v>
+      </c>
+      <c r="F17" s="158">
+        <v>0</v>
+      </c>
+      <c r="G17" s="158">
+        <v>0</v>
+      </c>
+      <c r="H17" s="158">
+        <v>0</v>
+      </c>
+      <c r="I17" s="158">
+        <v>0</v>
+      </c>
+      <c r="J17" s="158">
+        <v>0</v>
+      </c>
+      <c r="K17" s="158">
+        <v>0</v>
+      </c>
+      <c r="L17" s="158">
+        <v>0</v>
+      </c>
+      <c r="M17" s="158">
+        <v>0</v>
+      </c>
+      <c r="N17" s="158">
+        <v>0</v>
+      </c>
+      <c r="O17" s="158">
+        <v>0</v>
+      </c>
+      <c r="P17" s="158">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="158">
+        <v>0</v>
+      </c>
+      <c r="R17" s="158">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="169" t="s">
+        <v>492</v>
+      </c>
+      <c r="B19" s="158">
+        <f>SUM(B20,B21,B23)</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="167" t="s">
+        <v>521</v>
+      </c>
+      <c r="B20" s="158">
+        <f>SUM(C20:R20)</f>
+        <v>16</v>
+      </c>
+      <c r="C20" s="158">
+        <v>1</v>
+      </c>
+      <c r="D20" s="158">
+        <v>1</v>
+      </c>
+      <c r="E20" s="158">
+        <v>1</v>
+      </c>
+      <c r="F20" s="158">
+        <v>1</v>
+      </c>
+      <c r="G20" s="158">
+        <v>1</v>
+      </c>
+      <c r="H20" s="158">
+        <v>1</v>
+      </c>
+      <c r="I20" s="158">
+        <v>1</v>
+      </c>
+      <c r="J20" s="158">
+        <v>1</v>
+      </c>
+      <c r="K20" s="158">
+        <v>1</v>
+      </c>
+      <c r="L20" s="158">
+        <v>1</v>
+      </c>
+      <c r="M20" s="158">
+        <v>1</v>
+      </c>
+      <c r="N20" s="158">
+        <v>1</v>
+      </c>
+      <c r="O20" s="158">
+        <v>1</v>
+      </c>
+      <c r="P20" s="158">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="158">
+        <v>1</v>
+      </c>
+      <c r="R20" s="158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="169" t="s">
+        <v>493</v>
+      </c>
+      <c r="B21" s="158">
+        <f>SUM(C21:R21)</f>
+        <v>21</v>
+      </c>
+      <c r="C21" s="158">
+        <v>2</v>
+      </c>
+      <c r="D21" s="158">
+        <v>2</v>
+      </c>
+      <c r="E21" s="158">
+        <v>2</v>
+      </c>
+      <c r="F21" s="158">
+        <v>2</v>
+      </c>
+      <c r="G21" s="158">
+        <v>2</v>
+      </c>
+      <c r="H21" s="158">
+        <v>1</v>
+      </c>
+      <c r="I21" s="158">
+        <v>1</v>
+      </c>
+      <c r="J21" s="158">
+        <v>1</v>
+      </c>
+      <c r="K21" s="158">
+        <v>1</v>
+      </c>
+      <c r="L21" s="158">
+        <v>1</v>
+      </c>
+      <c r="M21" s="158">
+        <v>1</v>
+      </c>
+      <c r="N21" s="158">
+        <v>1</v>
+      </c>
+      <c r="O21" s="158">
+        <v>1</v>
+      </c>
+      <c r="P21" s="158">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="158">
+        <v>1</v>
+      </c>
+      <c r="R21" s="158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="169"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="169" t="s">
+        <v>494</v>
+      </c>
+      <c r="B23" s="158">
+        <f>SUM(C23:R23)</f>
+        <v>25</v>
+      </c>
+      <c r="C23" s="158">
+        <v>0</v>
+      </c>
+      <c r="D23" s="158">
+        <v>0</v>
+      </c>
+      <c r="E23" s="158">
+        <v>0</v>
+      </c>
+      <c r="F23" s="158">
+        <v>0</v>
+      </c>
+      <c r="G23" s="158">
+        <v>0</v>
+      </c>
+      <c r="H23" s="158">
+        <v>0</v>
+      </c>
+      <c r="I23" s="158">
+        <v>0</v>
+      </c>
+      <c r="J23" s="158">
+        <v>0</v>
+      </c>
+      <c r="K23" s="158">
+        <v>0</v>
+      </c>
+      <c r="L23" s="158">
+        <v>0</v>
+      </c>
+      <c r="M23" s="158">
+        <v>0</v>
+      </c>
+      <c r="N23" s="158">
+        <v>0</v>
+      </c>
+      <c r="O23" s="158">
+        <v>0</v>
+      </c>
+      <c r="P23" s="158">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="158">
+        <v>0</v>
+      </c>
+      <c r="R23" s="158">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="169"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="169" t="s">
+        <v>495</v>
+      </c>
+      <c r="B25" s="158">
+        <f>SUM(C25:R25)</f>
+        <v>5</v>
+      </c>
+      <c r="C25" s="158">
+        <v>1</v>
+      </c>
+      <c r="D25" s="158">
+        <v>1</v>
+      </c>
+      <c r="E25" s="158">
+        <v>1</v>
+      </c>
+      <c r="F25" s="158">
+        <v>1</v>
+      </c>
+      <c r="G25" s="158">
+        <v>1</v>
+      </c>
+      <c r="H25" s="158">
+        <v>0</v>
+      </c>
+      <c r="I25" s="158">
+        <v>0</v>
+      </c>
+      <c r="J25" s="158">
+        <v>0</v>
+      </c>
+      <c r="K25" s="158">
+        <v>0</v>
+      </c>
+      <c r="L25" s="158">
+        <v>0</v>
+      </c>
+      <c r="M25" s="158">
+        <v>0</v>
+      </c>
+      <c r="N25" s="158">
+        <v>0</v>
+      </c>
+      <c r="O25" s="158">
+        <v>0</v>
+      </c>
+      <c r="P25" s="158">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="158">
+        <v>0</v>
+      </c>
+      <c r="R25" s="158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="169"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="168" t="s">
+        <v>490</v>
+      </c>
+      <c r="B27" s="158">
+        <f>SUM(B29,B30)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="168"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="169" t="s">
+        <v>496</v>
+      </c>
+      <c r="B29" s="158">
+        <f>SUM(C29:R29)</f>
+        <v>26</v>
+      </c>
+      <c r="C29" s="158">
+        <v>3</v>
+      </c>
+      <c r="D29" s="158">
+        <v>3</v>
+      </c>
+      <c r="E29" s="158">
+        <v>3</v>
+      </c>
+      <c r="F29" s="158">
+        <v>3</v>
+      </c>
+      <c r="G29" s="158">
+        <v>3</v>
+      </c>
+      <c r="H29" s="158">
+        <v>1</v>
+      </c>
+      <c r="I29" s="158">
+        <v>1</v>
+      </c>
+      <c r="J29" s="158">
+        <v>1</v>
+      </c>
+      <c r="K29" s="158">
+        <v>1</v>
+      </c>
+      <c r="L29" s="158">
+        <v>1</v>
+      </c>
+      <c r="M29" s="158">
+        <v>1</v>
+      </c>
+      <c r="N29" s="158">
+        <v>1</v>
+      </c>
+      <c r="O29" s="158">
+        <v>1</v>
+      </c>
+      <c r="P29" s="158">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="158">
+        <v>1</v>
+      </c>
+      <c r="R29" s="158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="169" t="s">
+        <v>497</v>
+      </c>
+      <c r="B30" s="158">
+        <f>SUM(C30:R30)</f>
+        <v>26</v>
+      </c>
+      <c r="C30" s="158">
+        <v>3</v>
+      </c>
+      <c r="D30" s="158">
+        <v>3</v>
+      </c>
+      <c r="E30" s="158">
+        <v>3</v>
+      </c>
+      <c r="F30" s="158">
+        <v>3</v>
+      </c>
+      <c r="G30" s="158">
+        <v>3</v>
+      </c>
+      <c r="H30" s="158">
+        <v>1</v>
+      </c>
+      <c r="I30" s="158">
+        <v>1</v>
+      </c>
+      <c r="J30" s="158">
+        <v>1</v>
+      </c>
+      <c r="K30" s="158">
+        <v>1</v>
+      </c>
+      <c r="L30" s="158">
+        <v>1</v>
+      </c>
+      <c r="M30" s="158">
+        <v>1</v>
+      </c>
+      <c r="N30" s="158">
+        <v>1</v>
+      </c>
+      <c r="O30" s="158">
+        <v>1</v>
+      </c>
+      <c r="P30" s="158">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="158">
+        <v>1</v>
+      </c>
+      <c r="R30" s="158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="169"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="168" t="s">
+        <v>522</v>
+      </c>
+      <c r="B32" s="158">
+        <f>SUM(B4,B10,B27)</f>
+        <v>495</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4544,10 +5495,10 @@
       <c r="F25" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="I25" s="158" t="s">
+      <c r="I25" s="170" t="s">
         <v>370</v>
       </c>
-      <c r="J25" s="158"/>
+      <c r="J25" s="170"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
@@ -4565,8 +5516,8 @@
       <c r="F26" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="I26" s="159"/>
-      <c r="J26" s="159"/>
+      <c r="I26" s="171"/>
+      <c r="J26" s="171"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="12" t="s">
@@ -4756,12 +5707,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K39"/>
+  <dimension ref="B3:K70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4771,565 +5722,555 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="160" t="s">
-        <v>484</v>
-      </c>
-      <c r="C2" s="160"/>
-    </row>
-    <row r="3" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="165" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="166"/>
-      <c r="D5" s="167" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="168"/>
-      <c r="F5" s="169" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="170"/>
-      <c r="H5" s="171" t="s">
-        <v>382</v>
-      </c>
-      <c r="I5" s="172"/>
-      <c r="J5" s="173" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="174"/>
-    </row>
-    <row r="6" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="41" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="46" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" s="40" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="48" t="s">
-        <v>208</v>
-      </c>
-      <c r="C7" s="60" t="s">
-        <v>209</v>
-      </c>
-      <c r="D7" s="48" t="s">
-        <v>210</v>
-      </c>
-      <c r="E7" s="49" t="s">
-        <v>470</v>
-      </c>
-      <c r="F7" s="62" t="s">
-        <v>211</v>
-      </c>
-      <c r="G7" s="60" t="s">
-        <v>212</v>
-      </c>
-      <c r="H7" s="48" t="s">
-        <v>213</v>
-      </c>
-      <c r="I7" s="49" t="s">
-        <v>214</v>
-      </c>
-      <c r="J7" s="62" t="s">
-        <v>215</v>
-      </c>
-      <c r="K7" s="49" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="33" t="s">
-        <v>217</v>
-      </c>
-      <c r="C8" s="61" t="s">
-        <v>218</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>219</v>
-      </c>
-      <c r="E8" s="34" t="s">
-        <v>220</v>
-      </c>
-      <c r="F8" s="63" t="s">
-        <v>221</v>
-      </c>
-      <c r="G8" s="61" t="s">
-        <v>222</v>
-      </c>
-      <c r="H8" s="33" t="s">
-        <v>480</v>
-      </c>
-      <c r="I8" s="34" t="s">
-        <v>223</v>
-      </c>
-      <c r="J8" s="63" t="s">
-        <v>224</v>
-      </c>
-      <c r="K8" s="34" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="161" t="s">
-        <v>226</v>
-      </c>
-      <c r="C9" s="162"/>
-      <c r="D9" s="161" t="s">
-        <v>469</v>
-      </c>
-      <c r="E9" s="163"/>
-      <c r="F9" s="164" t="s">
-        <v>227</v>
-      </c>
-      <c r="G9" s="162"/>
-      <c r="H9" s="161" t="s">
-        <v>228</v>
-      </c>
-      <c r="I9" s="163"/>
-      <c r="J9" s="164" t="s">
-        <v>229</v>
-      </c>
-      <c r="K9" s="163"/>
-    </row>
-    <row r="10" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="185" t="s">
-        <v>230</v>
-      </c>
-      <c r="C10" s="186"/>
-      <c r="D10" s="185" t="s">
-        <v>231</v>
-      </c>
-      <c r="E10" s="187"/>
-      <c r="F10" s="188" t="s">
-        <v>471</v>
-      </c>
-      <c r="G10" s="186"/>
-      <c r="H10" s="185" t="s">
-        <v>465</v>
-      </c>
-      <c r="I10" s="187"/>
-      <c r="J10" s="188" t="s">
-        <v>232</v>
-      </c>
-      <c r="K10" s="187"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-    </row>
-    <row r="13" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="175" t="s">
-        <v>371</v>
-      </c>
-      <c r="C14" s="176"/>
-      <c r="D14" s="177" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="178"/>
-      <c r="F14" s="179" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" s="180"/>
-      <c r="H14" s="181" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14" s="182"/>
-      <c r="J14" s="183" t="s">
-        <v>17</v>
-      </c>
-      <c r="K14" s="184"/>
-    </row>
-    <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="53" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="54" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="55" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="56" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" s="57" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="J15" s="83" t="s">
-        <v>31</v>
-      </c>
-      <c r="K15" s="59" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="31" t="s">
-        <v>388</v>
-      </c>
-      <c r="C16" s="32" t="s">
-        <v>482</v>
-      </c>
-      <c r="D16" s="66" t="s">
-        <v>236</v>
-      </c>
-      <c r="E16" s="32" t="s">
-        <v>237</v>
-      </c>
-      <c r="F16" s="66" t="s">
-        <v>238</v>
-      </c>
-      <c r="G16" s="65" t="s">
-        <v>239</v>
-      </c>
-      <c r="H16" s="31" t="s">
-        <v>234</v>
-      </c>
-      <c r="I16" s="65" t="s">
-        <v>235</v>
-      </c>
-      <c r="J16" s="31"/>
-      <c r="K16" s="32" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="35" t="s">
-        <v>249</v>
-      </c>
-      <c r="C17" s="36" t="s">
-        <v>483</v>
-      </c>
-      <c r="D17" s="64" t="s">
-        <v>243</v>
-      </c>
-      <c r="E17" s="34" t="s">
-        <v>244</v>
-      </c>
-      <c r="F17" s="63" t="s">
-        <v>245</v>
-      </c>
-      <c r="G17" s="61" t="s">
-        <v>246</v>
-      </c>
-      <c r="H17" s="33" t="s">
-        <v>241</v>
-      </c>
-      <c r="I17" s="61" t="s">
-        <v>242</v>
-      </c>
-      <c r="J17" s="35"/>
-      <c r="K17" s="36" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="161" t="s">
-        <v>481</v>
-      </c>
-      <c r="C18" s="163"/>
-      <c r="D18" s="164" t="s">
-        <v>248</v>
-      </c>
-      <c r="E18" s="163"/>
-      <c r="F18" s="164" t="s">
-        <v>250</v>
-      </c>
-      <c r="G18" s="162"/>
-      <c r="H18" s="161" t="s">
-        <v>247</v>
-      </c>
-      <c r="I18" s="162"/>
-      <c r="J18" s="161" t="s">
-        <v>432</v>
-      </c>
-      <c r="K18" s="163"/>
-    </row>
-    <row r="19" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="185" t="s">
-        <v>253</v>
-      </c>
-      <c r="C19" s="187"/>
-      <c r="D19" s="188" t="s">
-        <v>252</v>
-      </c>
-      <c r="E19" s="187"/>
-      <c r="F19" s="188" t="s">
-        <v>254</v>
-      </c>
-      <c r="G19" s="186"/>
-      <c r="H19" s="185" t="s">
-        <v>251</v>
-      </c>
-      <c r="I19" s="186"/>
-      <c r="J19" s="185" t="s">
-        <v>468</v>
-      </c>
-      <c r="K19" s="187"/>
-    </row>
-    <row r="21" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="87" t="s">
-        <v>258</v>
-      </c>
-      <c r="E22" s="89" t="s">
-        <v>255</v>
-      </c>
-      <c r="F22" s="93" t="s">
-        <v>256</v>
-      </c>
-      <c r="G22" s="8"/>
-      <c r="I22" s="190" t="s">
-        <v>257</v>
-      </c>
-      <c r="J22" s="191"/>
-      <c r="K22" s="192"/>
-    </row>
-    <row r="23" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="81" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="88" t="s">
-        <v>288</v>
-      </c>
-      <c r="F23" s="82" t="s">
-        <v>35</v>
-      </c>
-      <c r="I23" s="84" t="s">
-        <v>259</v>
-      </c>
-      <c r="J23" s="85" t="s">
-        <v>260</v>
-      </c>
-      <c r="K23" s="86" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="69" t="s">
-        <v>472</v>
-      </c>
-      <c r="E24" s="31" t="s">
-        <v>262</v>
-      </c>
-      <c r="F24" s="73" t="s">
-        <v>263</v>
-      </c>
-      <c r="I24" s="72" t="s">
-        <v>264</v>
-      </c>
-      <c r="J24" s="77" t="s">
-        <v>265</v>
-      </c>
-      <c r="K24" s="76" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="70" t="s">
-        <v>272</v>
-      </c>
-      <c r="E25" s="33" t="s">
-        <v>267</v>
-      </c>
-      <c r="F25" s="74" t="s">
-        <v>268</v>
-      </c>
-      <c r="I25" s="78" t="s">
-        <v>269</v>
-      </c>
-      <c r="J25" s="79" t="s">
-        <v>270</v>
-      </c>
-      <c r="K25" s="9" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="70" t="s">
-        <v>278</v>
-      </c>
-      <c r="E26" s="33" t="s">
-        <v>273</v>
-      </c>
-      <c r="F26" s="74" t="s">
-        <v>274</v>
-      </c>
-      <c r="I26" s="78" t="s">
-        <v>275</v>
-      </c>
-      <c r="J26" s="79" t="s">
-        <v>276</v>
-      </c>
-      <c r="K26" s="10" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="71" t="s">
-        <v>283</v>
-      </c>
-      <c r="E27" s="33" t="s">
-        <v>279</v>
-      </c>
-      <c r="F27" s="75" t="s">
-        <v>280</v>
-      </c>
-      <c r="I27" s="78" t="s">
-        <v>281</v>
-      </c>
-      <c r="J27" s="9" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E28" s="67" t="s">
-        <v>284</v>
-      </c>
-      <c r="F28" s="68"/>
-      <c r="I28" s="80" t="s">
-        <v>285</v>
-      </c>
-      <c r="J28" s="9" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J29" s="71" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="113" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="111" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34" s="189"/>
-      <c r="D34" s="189"/>
-    </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C35"/>
       <c r="D35"/>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C36"/>
       <c r="D36"/>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C37"/>
       <c r="D37"/>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C38" s="189"/>
-      <c r="D38" s="189"/>
-    </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C39" s="189"/>
-      <c r="D39" s="189"/>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="204" t="s">
+        <v>484</v>
+      </c>
+      <c r="C38" s="204"/>
+    </row>
+    <row r="40" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40"/>
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="194" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="195"/>
+      <c r="D41" s="196" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="197"/>
+      <c r="F41" s="198" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" s="199"/>
+      <c r="H41" s="200" t="s">
+        <v>382</v>
+      </c>
+      <c r="I41" s="201"/>
+      <c r="J41" s="202" t="s">
+        <v>14</v>
+      </c>
+      <c r="K41" s="203"/>
+    </row>
+    <row r="42" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C42" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="E42" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="F42" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G42" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="H42" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="I42" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="J42" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="K42" s="40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="48" t="s">
+        <v>208</v>
+      </c>
+      <c r="C43" s="60" t="s">
+        <v>209</v>
+      </c>
+      <c r="D43" s="48" t="s">
+        <v>210</v>
+      </c>
+      <c r="E43" s="49" t="s">
+        <v>470</v>
+      </c>
+      <c r="F43" s="62" t="s">
+        <v>211</v>
+      </c>
+      <c r="G43" s="60" t="s">
+        <v>212</v>
+      </c>
+      <c r="H43" s="48" t="s">
+        <v>213</v>
+      </c>
+      <c r="I43" s="49" t="s">
+        <v>214</v>
+      </c>
+      <c r="J43" s="62" t="s">
+        <v>215</v>
+      </c>
+      <c r="K43" s="49" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B44" s="33" t="s">
+        <v>217</v>
+      </c>
+      <c r="C44" s="61" t="s">
+        <v>218</v>
+      </c>
+      <c r="D44" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="E44" s="34" t="s">
+        <v>220</v>
+      </c>
+      <c r="F44" s="63" t="s">
+        <v>221</v>
+      </c>
+      <c r="G44" s="61" t="s">
+        <v>222</v>
+      </c>
+      <c r="H44" s="33" t="s">
+        <v>480</v>
+      </c>
+      <c r="I44" s="34" t="s">
+        <v>223</v>
+      </c>
+      <c r="J44" s="63" t="s">
+        <v>224</v>
+      </c>
+      <c r="K44" s="34" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="176" t="s">
+        <v>226</v>
+      </c>
+      <c r="C45" s="178"/>
+      <c r="D45" s="176" t="s">
+        <v>469</v>
+      </c>
+      <c r="E45" s="177"/>
+      <c r="F45" s="179" t="s">
+        <v>227</v>
+      </c>
+      <c r="G45" s="178"/>
+      <c r="H45" s="176" t="s">
+        <v>228</v>
+      </c>
+      <c r="I45" s="177"/>
+      <c r="J45" s="179" t="s">
+        <v>229</v>
+      </c>
+      <c r="K45" s="177"/>
+    </row>
+    <row r="46" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="180" t="s">
+        <v>230</v>
+      </c>
+      <c r="C46" s="182"/>
+      <c r="D46" s="180" t="s">
+        <v>231</v>
+      </c>
+      <c r="E46" s="181"/>
+      <c r="F46" s="183" t="s">
+        <v>471</v>
+      </c>
+      <c r="G46" s="182"/>
+      <c r="H46" s="180" t="s">
+        <v>465</v>
+      </c>
+      <c r="I46" s="181"/>
+      <c r="J46" s="183" t="s">
+        <v>232</v>
+      </c>
+      <c r="K46" s="181"/>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B48"/>
+      <c r="C48"/>
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48"/>
+    </row>
+    <row r="49" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49"/>
+      <c r="C49"/>
+      <c r="D49"/>
+      <c r="E49"/>
+      <c r="F49"/>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B50" s="184" t="s">
+        <v>371</v>
+      </c>
+      <c r="C50" s="185"/>
+      <c r="D50" s="186" t="s">
+        <v>23</v>
+      </c>
+      <c r="E50" s="187"/>
+      <c r="F50" s="188" t="s">
+        <v>27</v>
+      </c>
+      <c r="G50" s="189"/>
+      <c r="H50" s="190" t="s">
+        <v>20</v>
+      </c>
+      <c r="I50" s="191"/>
+      <c r="J50" s="192" t="s">
+        <v>17</v>
+      </c>
+      <c r="K50" s="193"/>
+    </row>
+    <row r="51" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="C51" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="D51" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="E51" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="F51" s="55" t="s">
+        <v>33</v>
+      </c>
+      <c r="G51" s="56" t="s">
+        <v>34</v>
+      </c>
+      <c r="H51" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="I51" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="J51" s="83" t="s">
+        <v>31</v>
+      </c>
+      <c r="K51" s="59" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B52" s="31" t="s">
+        <v>388</v>
+      </c>
+      <c r="C52" s="32" t="s">
+        <v>482</v>
+      </c>
+      <c r="D52" s="66" t="s">
+        <v>236</v>
+      </c>
+      <c r="E52" s="32" t="s">
+        <v>237</v>
+      </c>
+      <c r="F52" s="66" t="s">
+        <v>238</v>
+      </c>
+      <c r="G52" s="65" t="s">
+        <v>239</v>
+      </c>
+      <c r="H52" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="I52" s="65" t="s">
+        <v>235</v>
+      </c>
+      <c r="J52" s="31"/>
+      <c r="K52" s="32" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B53" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="C53" s="36" t="s">
+        <v>483</v>
+      </c>
+      <c r="D53" s="64" t="s">
+        <v>243</v>
+      </c>
+      <c r="E53" s="34" t="s">
+        <v>244</v>
+      </c>
+      <c r="F53" s="63" t="s">
+        <v>245</v>
+      </c>
+      <c r="G53" s="61" t="s">
+        <v>246</v>
+      </c>
+      <c r="H53" s="33" t="s">
+        <v>241</v>
+      </c>
+      <c r="I53" s="61" t="s">
+        <v>242</v>
+      </c>
+      <c r="J53" s="35"/>
+      <c r="K53" s="36" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B54" s="176" t="s">
+        <v>481</v>
+      </c>
+      <c r="C54" s="177"/>
+      <c r="D54" s="179" t="s">
+        <v>248</v>
+      </c>
+      <c r="E54" s="177"/>
+      <c r="F54" s="179" t="s">
+        <v>250</v>
+      </c>
+      <c r="G54" s="178"/>
+      <c r="H54" s="176" t="s">
+        <v>247</v>
+      </c>
+      <c r="I54" s="178"/>
+      <c r="J54" s="176" t="s">
+        <v>432</v>
+      </c>
+      <c r="K54" s="177"/>
+    </row>
+    <row r="55" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="180" t="s">
+        <v>253</v>
+      </c>
+      <c r="C55" s="181"/>
+      <c r="D55" s="183" t="s">
+        <v>252</v>
+      </c>
+      <c r="E55" s="181"/>
+      <c r="F55" s="183" t="s">
+        <v>254</v>
+      </c>
+      <c r="G55" s="182"/>
+      <c r="H55" s="180" t="s">
+        <v>251</v>
+      </c>
+      <c r="I55" s="182"/>
+      <c r="J55" s="180" t="s">
+        <v>468</v>
+      </c>
+      <c r="K55" s="181"/>
+    </row>
+    <row r="57" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B58" s="87" t="s">
+        <v>258</v>
+      </c>
+      <c r="E58" s="89" t="s">
+        <v>255</v>
+      </c>
+      <c r="F58" s="93" t="s">
+        <v>256</v>
+      </c>
+      <c r="G58" s="8"/>
+      <c r="I58" s="173" t="s">
+        <v>257</v>
+      </c>
+      <c r="J58" s="174"/>
+      <c r="K58" s="175"/>
+    </row>
+    <row r="59" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="81" t="s">
+        <v>35</v>
+      </c>
+      <c r="E59" s="88" t="s">
+        <v>288</v>
+      </c>
+      <c r="F59" s="82" t="s">
+        <v>35</v>
+      </c>
+      <c r="I59" s="84" t="s">
+        <v>259</v>
+      </c>
+      <c r="J59" s="85" t="s">
+        <v>260</v>
+      </c>
+      <c r="K59" s="86" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B60" s="69" t="s">
+        <v>472</v>
+      </c>
+      <c r="E60" s="31" t="s">
+        <v>262</v>
+      </c>
+      <c r="F60" s="73" t="s">
+        <v>263</v>
+      </c>
+      <c r="I60" s="72" t="s">
+        <v>264</v>
+      </c>
+      <c r="J60" s="77" t="s">
+        <v>265</v>
+      </c>
+      <c r="K60" s="76" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B61" s="70" t="s">
+        <v>272</v>
+      </c>
+      <c r="E61" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="F61" s="74" t="s">
+        <v>268</v>
+      </c>
+      <c r="I61" s="78" t="s">
+        <v>269</v>
+      </c>
+      <c r="J61" s="79" t="s">
+        <v>270</v>
+      </c>
+      <c r="K61" s="9" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="70" t="s">
+        <v>278</v>
+      </c>
+      <c r="E62" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="F62" s="74" t="s">
+        <v>274</v>
+      </c>
+      <c r="I62" s="78" t="s">
+        <v>275</v>
+      </c>
+      <c r="J62" s="79" t="s">
+        <v>276</v>
+      </c>
+      <c r="K62" s="10" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="71" t="s">
+        <v>283</v>
+      </c>
+      <c r="E63" s="33" t="s">
+        <v>279</v>
+      </c>
+      <c r="F63" s="75" t="s">
+        <v>280</v>
+      </c>
+      <c r="I63" s="78" t="s">
+        <v>281</v>
+      </c>
+      <c r="J63" s="9" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="64" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E64" s="67" t="s">
+        <v>284</v>
+      </c>
+      <c r="F64" s="68"/>
+      <c r="I64" s="80" t="s">
+        <v>285</v>
+      </c>
+      <c r="J64" s="9" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J65" s="71" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="67" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="113" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="111" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C70" s="172"/>
+      <c r="D70" s="172"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
+  <mergeCells count="33">
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="I58:K58"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="J55:K55"/>
+    <mergeCell ref="F55:G55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E92"/>
   <sheetViews>
@@ -5391,7 +6332,7 @@
       <c r="C7" s="116" t="s">
         <v>297</v>
       </c>
-      <c r="D7" s="193" t="s">
+      <c r="D7" s="205" t="s">
         <v>452</v>
       </c>
     </row>
@@ -5402,7 +6343,7 @@
       <c r="C8" s="116" t="s">
         <v>299</v>
       </c>
-      <c r="D8" s="194"/>
+      <c r="D8" s="206"/>
     </row>
     <row r="9" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="108" t="s">
@@ -5411,7 +6352,7 @@
       <c r="C9" s="116" t="s">
         <v>301</v>
       </c>
-      <c r="D9" s="194"/>
+      <c r="D9" s="206"/>
     </row>
     <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="108" t="s">
@@ -5420,7 +6361,7 @@
       <c r="C10" s="116" t="s">
         <v>302</v>
       </c>
-      <c r="D10" s="194"/>
+      <c r="D10" s="206"/>
     </row>
     <row r="11" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="108" t="s">
@@ -5429,7 +6370,7 @@
       <c r="C11" s="116" t="s">
         <v>304</v>
       </c>
-      <c r="D11" s="194"/>
+      <c r="D11" s="206"/>
     </row>
     <row r="12" spans="2:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B12" s="108" t="s">
@@ -5438,7 +6379,7 @@
       <c r="C12" s="116" t="s">
         <v>306</v>
       </c>
-      <c r="D12" s="194"/>
+      <c r="D12" s="206"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="108" t="s">
@@ -5447,7 +6388,7 @@
       <c r="C13" s="116" t="s">
         <v>308</v>
       </c>
-      <c r="D13" s="194"/>
+      <c r="D13" s="206"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="108" t="s">
@@ -5456,7 +6397,7 @@
       <c r="C14" s="116" t="s">
         <v>310</v>
       </c>
-      <c r="D14" s="194"/>
+      <c r="D14" s="206"/>
     </row>
     <row r="15" spans="2:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="109" t="s">
@@ -5465,7 +6406,7 @@
       <c r="C15" s="114" t="s">
         <v>312</v>
       </c>
-      <c r="D15" s="195"/>
+      <c r="D15" s="207"/>
     </row>
     <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5517,7 +6458,7 @@
       <c r="C24" s="116" t="s">
         <v>323</v>
       </c>
-      <c r="D24" s="193" t="s">
+      <c r="D24" s="205" t="s">
         <v>324</v>
       </c>
     </row>
@@ -5528,7 +6469,7 @@
       <c r="C25" s="116" t="s">
         <v>326</v>
       </c>
-      <c r="D25" s="194"/>
+      <c r="D25" s="206"/>
     </row>
     <row r="26" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="108" t="s">
@@ -5537,7 +6478,7 @@
       <c r="C26" s="116" t="s">
         <v>328</v>
       </c>
-      <c r="D26" s="197"/>
+      <c r="D26" s="209"/>
     </row>
     <row r="27" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="108" t="s">
@@ -5635,7 +6576,7 @@
       <c r="C37" s="149" t="s">
         <v>349</v>
       </c>
-      <c r="D37" s="196" t="s">
+      <c r="D37" s="208" t="s">
         <v>350</v>
       </c>
     </row>
@@ -5646,7 +6587,7 @@
       <c r="C38" s="116" t="s">
         <v>352</v>
       </c>
-      <c r="D38" s="197"/>
+      <c r="D38" s="209"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="108"/>
@@ -5715,7 +6656,7 @@
         <v>354</v>
       </c>
       <c r="C51" s="149"/>
-      <c r="D51" s="196" t="s">
+      <c r="D51" s="208" t="s">
         <v>355</v>
       </c>
     </row>
@@ -5724,14 +6665,14 @@
         <v>356</v>
       </c>
       <c r="C52" s="116"/>
-      <c r="D52" s="194"/>
+      <c r="D52" s="206"/>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="108" t="s">
         <v>357</v>
       </c>
       <c r="C53" s="116"/>
-      <c r="D53" s="197"/>
+      <c r="D53" s="209"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="108"/>
@@ -5814,7 +6755,7 @@
       <c r="C66" s="116" t="s">
         <v>464</v>
       </c>
-      <c r="D66" s="196" t="s">
+      <c r="D66" s="208" t="s">
         <v>462</v>
       </c>
     </row>
@@ -5825,7 +6766,7 @@
       <c r="C67" s="116" t="s">
         <v>458</v>
       </c>
-      <c r="D67" s="194"/>
+      <c r="D67" s="206"/>
     </row>
     <row r="68" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="108" t="s">
@@ -5834,7 +6775,7 @@
       <c r="C68" s="116" t="s">
         <v>459</v>
       </c>
-      <c r="D68" s="194"/>
+      <c r="D68" s="206"/>
     </row>
     <row r="69" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B69" s="108" t="s">
@@ -5843,7 +6784,7 @@
       <c r="C69" s="116" t="s">
         <v>460</v>
       </c>
-      <c r="D69" s="194"/>
+      <c r="D69" s="206"/>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="108" t="s">
@@ -5852,7 +6793,7 @@
       <c r="C70" s="116" t="s">
         <v>461</v>
       </c>
-      <c r="D70" s="197"/>
+      <c r="D70" s="209"/>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="108"/>
@@ -5883,19 +6824,19 @@
     <row r="80" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B80" s="95"/>
       <c r="C80" s="95"/>
-      <c r="D80" s="198"/>
+      <c r="D80" s="210"/>
       <c r="E80" s="95"/>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" s="95"/>
       <c r="C81" s="95"/>
-      <c r="D81" s="198"/>
+      <c r="D81" s="210"/>
       <c r="E81" s="95"/>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="95"/>
       <c r="C82" s="95"/>
-      <c r="D82" s="198"/>
+      <c r="D82" s="210"/>
       <c r="E82" s="95"/>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
@@ -5971,7 +6912,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H37"/>
   <sheetViews>

</xml_diff>

<commit_message>
Changes to Champion Colors
Garen and Galio to Demacia (iconic)
Quinn to W, Ezreal to W/U, Orianna to Esper
</commit_message>
<xml_diff>
--- a/DesignDoc.xlsx
+++ b/DesignDoc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4815" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4815" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Factions" sheetId="6" r:id="rId1"/>
@@ -3275,6 +3275,93 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3283,93 +3370,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4188,7 +4188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
@@ -4991,8 +4991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5126,7 +5126,7 @@
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>69</v>
@@ -5231,7 +5231,7 @@
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>40</v>
@@ -5255,7 +5255,7 @@
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="12" t="s">
-        <v>65</v>
+        <v>161</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>100</v>
@@ -5348,7 +5348,7 @@
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
-        <v>139</v>
+        <v>65</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>140</v>
@@ -5580,7 +5580,7 @@
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="12" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>162</v>
@@ -5736,10 +5736,10 @@
       <c r="D37"/>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B38" s="204" t="s">
+      <c r="B38" s="172" t="s">
         <v>484</v>
       </c>
-      <c r="C38" s="204"/>
+      <c r="C38" s="172"/>
     </row>
     <row r="40" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40"/>
@@ -5749,26 +5749,26 @@
       <c r="F40"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B41" s="194" t="s">
+      <c r="B41" s="177" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="195"/>
-      <c r="D41" s="196" t="s">
+      <c r="C41" s="178"/>
+      <c r="D41" s="179" t="s">
         <v>6</v>
       </c>
-      <c r="E41" s="197"/>
-      <c r="F41" s="198" t="s">
+      <c r="E41" s="180"/>
+      <c r="F41" s="181" t="s">
         <v>9</v>
       </c>
-      <c r="G41" s="199"/>
-      <c r="H41" s="200" t="s">
+      <c r="G41" s="182"/>
+      <c r="H41" s="183" t="s">
         <v>382</v>
       </c>
-      <c r="I41" s="201"/>
-      <c r="J41" s="202" t="s">
+      <c r="I41" s="184"/>
+      <c r="J41" s="185" t="s">
         <v>14</v>
       </c>
-      <c r="K41" s="203"/>
+      <c r="K41" s="186"/>
     </row>
     <row r="42" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="39" t="s">
@@ -5867,48 +5867,48 @@
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B45" s="176" t="s">
+      <c r="B45" s="173" t="s">
         <v>226</v>
       </c>
-      <c r="C45" s="178"/>
-      <c r="D45" s="176" t="s">
+      <c r="C45" s="174"/>
+      <c r="D45" s="173" t="s">
         <v>469</v>
       </c>
-      <c r="E45" s="177"/>
-      <c r="F45" s="179" t="s">
+      <c r="E45" s="175"/>
+      <c r="F45" s="176" t="s">
         <v>227</v>
       </c>
-      <c r="G45" s="178"/>
-      <c r="H45" s="176" t="s">
+      <c r="G45" s="174"/>
+      <c r="H45" s="173" t="s">
         <v>228</v>
       </c>
-      <c r="I45" s="177"/>
-      <c r="J45" s="179" t="s">
+      <c r="I45" s="175"/>
+      <c r="J45" s="176" t="s">
         <v>229</v>
       </c>
-      <c r="K45" s="177"/>
+      <c r="K45" s="175"/>
     </row>
     <row r="46" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="180" t="s">
+      <c r="B46" s="197" t="s">
         <v>230</v>
       </c>
-      <c r="C46" s="182"/>
-      <c r="D46" s="180" t="s">
+      <c r="C46" s="198"/>
+      <c r="D46" s="197" t="s">
         <v>231</v>
       </c>
-      <c r="E46" s="181"/>
-      <c r="F46" s="183" t="s">
+      <c r="E46" s="199"/>
+      <c r="F46" s="200" t="s">
         <v>471</v>
       </c>
-      <c r="G46" s="182"/>
-      <c r="H46" s="180" t="s">
+      <c r="G46" s="198"/>
+      <c r="H46" s="197" t="s">
         <v>465</v>
       </c>
-      <c r="I46" s="181"/>
-      <c r="J46" s="183" t="s">
+      <c r="I46" s="199"/>
+      <c r="J46" s="200" t="s">
         <v>232</v>
       </c>
-      <c r="K46" s="181"/>
+      <c r="K46" s="199"/>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48"/>
@@ -5925,26 +5925,26 @@
       <c r="F49"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B50" s="184" t="s">
+      <c r="B50" s="187" t="s">
         <v>371</v>
       </c>
-      <c r="C50" s="185"/>
-      <c r="D50" s="186" t="s">
+      <c r="C50" s="188"/>
+      <c r="D50" s="189" t="s">
         <v>23</v>
       </c>
-      <c r="E50" s="187"/>
-      <c r="F50" s="188" t="s">
+      <c r="E50" s="190"/>
+      <c r="F50" s="191" t="s">
         <v>27</v>
       </c>
-      <c r="G50" s="189"/>
-      <c r="H50" s="190" t="s">
+      <c r="G50" s="192"/>
+      <c r="H50" s="193" t="s">
         <v>20</v>
       </c>
-      <c r="I50" s="191"/>
-      <c r="J50" s="192" t="s">
+      <c r="I50" s="194"/>
+      <c r="J50" s="195" t="s">
         <v>17</v>
       </c>
-      <c r="K50" s="193"/>
+      <c r="K50" s="196"/>
     </row>
     <row r="51" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="51" t="s">
@@ -6039,48 +6039,48 @@
       </c>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B54" s="176" t="s">
+      <c r="B54" s="173" t="s">
         <v>481</v>
       </c>
-      <c r="C54" s="177"/>
-      <c r="D54" s="179" t="s">
+      <c r="C54" s="175"/>
+      <c r="D54" s="176" t="s">
         <v>248</v>
       </c>
-      <c r="E54" s="177"/>
-      <c r="F54" s="179" t="s">
+      <c r="E54" s="175"/>
+      <c r="F54" s="176" t="s">
         <v>250</v>
       </c>
-      <c r="G54" s="178"/>
-      <c r="H54" s="176" t="s">
+      <c r="G54" s="174"/>
+      <c r="H54" s="173" t="s">
         <v>247</v>
       </c>
-      <c r="I54" s="178"/>
-      <c r="J54" s="176" t="s">
+      <c r="I54" s="174"/>
+      <c r="J54" s="173" t="s">
         <v>432</v>
       </c>
-      <c r="K54" s="177"/>
+      <c r="K54" s="175"/>
     </row>
     <row r="55" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="180" t="s">
+      <c r="B55" s="197" t="s">
         <v>253</v>
       </c>
-      <c r="C55" s="181"/>
-      <c r="D55" s="183" t="s">
+      <c r="C55" s="199"/>
+      <c r="D55" s="200" t="s">
         <v>252</v>
       </c>
-      <c r="E55" s="181"/>
-      <c r="F55" s="183" t="s">
+      <c r="E55" s="199"/>
+      <c r="F55" s="200" t="s">
         <v>254</v>
       </c>
-      <c r="G55" s="182"/>
-      <c r="H55" s="180" t="s">
+      <c r="G55" s="198"/>
+      <c r="H55" s="197" t="s">
         <v>251</v>
       </c>
-      <c r="I55" s="182"/>
-      <c r="J55" s="180" t="s">
+      <c r="I55" s="198"/>
+      <c r="J55" s="197" t="s">
         <v>468</v>
       </c>
-      <c r="K55" s="181"/>
+      <c r="K55" s="199"/>
     </row>
     <row r="57" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
@@ -6094,11 +6094,11 @@
         <v>256</v>
       </c>
       <c r="G58" s="8"/>
-      <c r="I58" s="173" t="s">
+      <c r="I58" s="202" t="s">
         <v>257</v>
       </c>
-      <c r="J58" s="174"/>
-      <c r="K58" s="175"/>
+      <c r="J58" s="203"/>
+      <c r="K58" s="204"/>
     </row>
     <row r="59" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="81" t="s">
@@ -6226,32 +6226,11 @@
       </c>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C70" s="172"/>
-      <c r="D70" s="172"/>
+      <c r="C70" s="201"/>
+      <c r="D70" s="201"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="J46:K46"/>
     <mergeCell ref="C70:D70"/>
     <mergeCell ref="I58:K58"/>
     <mergeCell ref="B54:C54"/>
@@ -6264,6 +6243,27 @@
     <mergeCell ref="D55:E55"/>
     <mergeCell ref="J55:K55"/>
     <mergeCell ref="F55:G55"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H45:I45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added set skeleton document
Minor tweaks to void and demacia
</commit_message>
<xml_diff>
--- a/DesignDoc.xlsx
+++ b/DesignDoc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4815" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4815" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Factions" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="533">
   <si>
     <t>Description</t>
   </si>
@@ -1338,12 +1338,6 @@
     <t>Rune</t>
   </si>
   <si>
-    <t>Artifact Enchantment</t>
-  </si>
-  <si>
-    <t>Counts as both an artifact and an enchantment.</t>
-  </si>
-  <si>
     <t>Rune for each Keystone in LoL.
 Only apply to certain classes (Fighter, Mage, Tank, etc.)</t>
   </si>
@@ -1501,9 +1495,6 @@
   </si>
   <si>
     <t>Infectious Voidling</t>
-  </si>
-  <si>
-    <t>* Unsure whether to use these or not</t>
   </si>
   <si>
     <t>Buff</t>
@@ -1676,6 +1667,52 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Unsure about whether it should prevent combat damage from that creature as well (for use as a combat trick).</t>
+  </si>
+  <si>
+    <t>Summoner</t>
+  </si>
+  <si>
+    <t>You may start the game with up to two Summoner cards in your command zone. Your maximum hand size is reduced by  the number of Summoner cards in your command zone. You may cast Summoner spells from your command zone if you pay 2 more to cast it.</t>
+  </si>
+  <si>
+    <t>Even distribution across factions, cards can be run in the '99'
+or
+Mono-colored cycle, cards can be run in the '99'
+or
+Summoners are colorless so that any deck can run it, would have to be pretty severly overcosted</t>
+  </si>
+  <si>
+    <t>Ability on some Instants/Sorceries that allow them to essentially start the game in hand.</t>
+  </si>
+  <si>
+    <t>Objective</t>
+  </si>
+  <si>
+    <t>Meta type that sits in command zone and provides emminence abilities for champions</t>
+  </si>
+  <si>
+    <t>Inhibitors, The Nexus, Baron Nashor, Twisted Treeline Altars.</t>
+  </si>
+  <si>
+    <t>Each player may start the game with one Keystone rune in the command zone.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New attackable permanent type.
+Provide static bonuses at the risk of having an opponent capture it for a reward.
+</t>
+  </si>
+  <si>
+    <t>Captures is new keyword that means whoever dealt the killing blow.</t>
+  </si>
+  <si>
+    <t>* Unsure whether to use these or not
+** Pretty sure now, not going to use..</t>
+  </si>
+  <si>
+    <t>Krugs</t>
   </si>
 </sst>
 </file>
@@ -2764,7 +2801,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="211">
+  <cellXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3269,99 +3306,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3372,6 +3323,93 @@
     <xf numFmtId="0" fontId="1" fillId="33" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3389,6 +3427,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3687,21 +3728,21 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="95"/>
-    <col min="2" max="2" width="14.7109375" style="95" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="27.7109375" style="95" customWidth="1"/>
-    <col min="6" max="6" width="91.85546875" style="95" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="95"/>
+    <col min="1" max="1" width="9.1328125" style="95"/>
+    <col min="2" max="2" width="14.73046875" style="95" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="27.73046875" style="95" customWidth="1"/>
+    <col min="6" max="6" width="91.86328125" style="95" customWidth="1"/>
+    <col min="7" max="16384" width="9.1328125" style="95"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="94"/>
       <c r="B1" s="94"/>
       <c r="C1" s="94"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="94"/>
       <c r="B2" s="90" t="s">
         <v>369</v>
@@ -3719,7 +3760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="94"/>
       <c r="B3" s="117" t="s">
         <v>3</v>
@@ -3731,13 +3772,13 @@
         <v>402</v>
       </c>
       <c r="E3" s="98" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="F3" s="99" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="94"/>
       <c r="B4" s="118" t="s">
         <v>6</v>
@@ -3749,13 +3790,13 @@
         <v>384</v>
       </c>
       <c r="E4" s="96" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="F4" s="100" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="94"/>
       <c r="B5" s="119" t="s">
         <v>9</v>
@@ -3767,13 +3808,13 @@
         <v>404</v>
       </c>
       <c r="E5" s="97" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="F5" s="101" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="94"/>
       <c r="B6" s="120" t="s">
         <v>11</v>
@@ -3788,10 +3829,10 @@
         <v>392</v>
       </c>
       <c r="F6" s="100" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="94"/>
       <c r="B7" s="121" t="s">
         <v>14</v>
@@ -3809,7 +3850,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="94"/>
       <c r="B8" s="122" t="s">
         <v>371</v>
@@ -3827,7 +3868,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="94"/>
       <c r="B9" s="123" t="s">
         <v>23</v>
@@ -3839,13 +3880,13 @@
         <v>401</v>
       </c>
       <c r="E9" s="96" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="F9" s="100" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="94"/>
       <c r="B10" s="124" t="s">
         <v>27</v>
@@ -3860,10 +3901,10 @@
         <v>390</v>
       </c>
       <c r="F10" s="101" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="94"/>
       <c r="B11" s="125" t="s">
         <v>20</v>
@@ -3881,7 +3922,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="94"/>
       <c r="B12" s="126" t="s">
         <v>17</v>
@@ -3893,27 +3934,27 @@
         <v>407</v>
       </c>
       <c r="E12" s="96" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="F12" s="100" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B13" s="127" t="s">
         <v>258</v>
       </c>
       <c r="C13" s="114" t="s">
+        <v>441</v>
+      </c>
+      <c r="D13" s="102" t="s">
+        <v>434</v>
+      </c>
+      <c r="E13" s="102" t="s">
+        <v>483</v>
+      </c>
+      <c r="F13" s="103" t="s">
         <v>443</v>
-      </c>
-      <c r="D13" s="102" t="s">
-        <v>436</v>
-      </c>
-      <c r="E13" s="102" t="s">
-        <v>486</v>
-      </c>
-      <c r="F13" s="103" t="s">
-        <v>445</v>
       </c>
     </row>
   </sheetData>
@@ -3923,25 +3964,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="5" width="52.42578125" customWidth="1"/>
-    <col min="6" max="7" width="48.42578125" customWidth="1"/>
-    <col min="17" max="18" width="18.28515625" customWidth="1"/>
-    <col min="19" max="21" width="48.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.265625" customWidth="1"/>
+    <col min="3" max="5" width="52.3984375" customWidth="1"/>
+    <col min="6" max="7" width="48.3984375" customWidth="1"/>
+    <col min="17" max="18" width="18.265625" customWidth="1"/>
+    <col min="19" max="21" width="48.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="90" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C2" s="91" t="s">
         <v>0</v>
@@ -3953,7 +3994,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B3" s="107" t="s">
         <v>419</v>
       </c>
@@ -3964,218 +4005,248 @@
         <v>421</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B4" s="109" t="s">
         <v>422</v>
       </c>
       <c r="C4" s="106" t="s">
+        <v>526</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>528</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>423</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>424</v>
-      </c>
-      <c r="E4" s="7" t="s">
+    </row>
+    <row r="5" spans="2:5" s="170" customFormat="1" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B5" s="109" t="s">
+        <v>525</v>
+      </c>
+      <c r="C5" s="106" t="s">
+        <v>529</v>
+      </c>
+      <c r="D5" s="212" t="s">
+        <v>530</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" s="170" customFormat="1" ht="85.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="109" t="s">
+        <v>521</v>
+      </c>
+      <c r="C6" s="106" t="s">
+        <v>524</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="8" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B8" s="90" t="s">
+        <v>428</v>
+      </c>
+      <c r="C8" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B9" s="107" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="104" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B10" s="108" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="105" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="2:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B11" s="108" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="105" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="90" t="s">
-        <v>430</v>
-      </c>
-      <c r="C6" s="91" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B7" s="107" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="104" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="108" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="105" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="108" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="105" t="s">
-        <v>427</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="108" t="s">
+    <row r="12" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B12" s="108" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="105" t="s">
+      <c r="C12" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="108" t="s">
+      <c r="E12" s="5" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B13" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="105" t="s">
+      <c r="C13" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="108" t="s">
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B14" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="105" t="s">
+      <c r="C14" s="105" t="s">
         <v>19</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B13" s="108" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="105" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B14" s="108" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="105" t="s">
-        <v>29</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B15" s="108" t="s">
-        <v>439</v>
+        <v>24</v>
       </c>
       <c r="C15" s="105" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="B16" s="108" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="105" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B17" s="108" t="s">
         <v>437</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="C17" s="105" t="s">
+        <v>435</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>438</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B16" s="108" t="s">
+    </row>
+    <row r="18" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B18" s="108" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="105" t="s">
+      <c r="C18" s="105" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="109" t="s">
-        <v>433</v>
-      </c>
-      <c r="C17" s="106" t="s">
-        <v>434</v>
-      </c>
-      <c r="D17" s="6" t="s">
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" ht="85.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B19" s="109" t="s">
+        <v>431</v>
+      </c>
+      <c r="C19" s="106" t="s">
+        <v>432</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E19" s="7" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="156"/>
-      <c r="B19" s="156"/>
-      <c r="C19" s="157" t="s">
+    <row r="21" spans="1:5" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="156"/>
+      <c r="B21" s="156"/>
+      <c r="C21" s="157" t="s">
+        <v>531</v>
+      </c>
+      <c r="D21" s="156"/>
+    </row>
+    <row r="22" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A22" s="156"/>
+      <c r="B22" s="90" t="s">
+        <v>427</v>
+      </c>
+      <c r="C22" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="156"/>
+      <c r="B23" s="107" t="s">
+        <v>471</v>
+      </c>
+      <c r="C23" s="104" t="s">
+        <v>474</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A24" s="156"/>
+      <c r="B24" s="109" t="s">
+        <v>472</v>
+      </c>
+      <c r="C24" s="106" t="s">
         <v>473</v>
       </c>
-      <c r="D19" s="156"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="156"/>
-      <c r="B20" s="90" t="s">
-        <v>429</v>
-      </c>
-      <c r="C20" s="91" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="29" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="156"/>
-      <c r="B21" s="107" t="s">
-        <v>474</v>
-      </c>
-      <c r="C21" s="104" t="s">
-        <v>477</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="156"/>
-      <c r="B22" s="109" t="s">
+      <c r="D24" s="6" t="s">
         <v>475</v>
-      </c>
-      <c r="C22" s="106" t="s">
-        <v>476</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>478</v>
       </c>
     </row>
   </sheetData>
@@ -4188,25 +4259,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="15" style="167" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="158" customWidth="1"/>
-    <col min="3" max="18" width="20.140625" style="158" customWidth="1"/>
-    <col min="19" max="16384" width="16.85546875" style="158"/>
+    <col min="2" max="2" width="12.59765625" style="158" customWidth="1"/>
+    <col min="3" max="18" width="20.1328125" style="158" customWidth="1"/>
+    <col min="19" max="16384" width="16.86328125" style="158"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="1:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="168" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B2" s="163" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="C2" s="128" t="s">
         <v>30</v>
@@ -4257,118 +4328,118 @@
         <v>258</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" s="168"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4" s="168" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B4" s="158">
         <f>SUM(B7,B6,B8)</f>
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" s="169"/>
       <c r="C5" s="163"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" s="169" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B6" s="158">
         <v>5</v>
       </c>
       <c r="C6" s="158" t="s">
+        <v>497</v>
+      </c>
+      <c r="D6" s="158" t="s">
+        <v>498</v>
+      </c>
+      <c r="E6" s="158" t="s">
+        <v>499</v>
+      </c>
+      <c r="F6" s="158" t="s">
         <v>500</v>
       </c>
-      <c r="D6" s="158" t="s">
+      <c r="G6" s="158" t="s">
         <v>501</v>
       </c>
-      <c r="E6" s="158" t="s">
-        <v>502</v>
-      </c>
-      <c r="F6" s="158" t="s">
-        <v>503</v>
-      </c>
-      <c r="G6" s="158" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" s="169" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="B7" s="158">
         <v>10</v>
       </c>
       <c r="H7" s="158" t="s">
+        <v>504</v>
+      </c>
+      <c r="I7" s="158" t="s">
+        <v>505</v>
+      </c>
+      <c r="J7" s="158" t="s">
+        <v>506</v>
+      </c>
+      <c r="K7" s="158" t="s">
         <v>507</v>
       </c>
-      <c r="I7" s="158" t="s">
+      <c r="L7" s="158" t="s">
+        <v>509</v>
+      </c>
+      <c r="M7" s="158" t="s">
         <v>508</v>
       </c>
-      <c r="J7" s="158" t="s">
-        <v>509</v>
-      </c>
-      <c r="K7" s="158" t="s">
+      <c r="N7" s="158" t="s">
         <v>510</v>
       </c>
-      <c r="L7" s="158" t="s">
+      <c r="O7" s="158" t="s">
         <v>512</v>
       </c>
-      <c r="M7" s="158" t="s">
+      <c r="P7" s="158" t="s">
         <v>511</v>
       </c>
-      <c r="N7" s="158" t="s">
+      <c r="Q7" s="158" t="s">
         <v>513</v>
       </c>
-      <c r="O7" s="158" t="s">
-        <v>515</v>
-      </c>
-      <c r="P7" s="158" t="s">
+      <c r="R7" s="158" t="s">
         <v>514</v>
       </c>
-      <c r="Q7" s="158" t="s">
-        <v>516</v>
-      </c>
-      <c r="R7" s="158" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" s="169" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" s="168"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10" s="168" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="B10" s="158">
         <f>SUM(B12,B14,B16,B19,B23,B25,-B23, -B23)</f>
         <v>428</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11" s="168"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A12" s="169" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="B12" s="158">
         <f>SUM(B13,B14)</f>
         <v>233</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A13" s="167" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="B13" s="158">
         <f>SUM(C13:R13)</f>
@@ -4423,7 +4494,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A14" s="169" t="s">
         <v>188</v>
       </c>
@@ -4480,12 +4551,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A15" s="169"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A16" s="169" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B16" s="158">
         <f>SUM(C16:R16,B17, B23)</f>
@@ -4540,7 +4611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A17" s="169" t="s">
         <v>313</v>
       </c>
@@ -4597,18 +4668,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A19" s="169" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B19" s="158">
         <f>SUM(B20,B21,B23)</f>
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A20" s="167" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B20" s="158">
         <f>SUM(C20:R20)</f>
@@ -4663,9 +4734,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A21" s="169" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B21" s="158">
         <f>SUM(C21:R21)</f>
@@ -4720,12 +4791,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A22" s="169"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A23" s="169" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B23" s="158">
         <f>SUM(C23:R23)</f>
@@ -4780,12 +4851,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A24" s="169"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A25" s="169" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B25" s="158">
         <f>SUM(C25:R25)</f>
@@ -4840,24 +4911,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A26" s="169"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A27" s="168" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="B27" s="158">
         <f>SUM(B29,B30)</f>
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A28" s="168"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A29" s="169" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B29" s="158">
         <f>SUM(C29:R29)</f>
@@ -4912,9 +4983,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A30" s="169" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B30" s="158">
         <f>SUM(C30:R30)</f>
@@ -4969,12 +5040,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A31" s="169"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A32" s="168" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="B32" s="158">
         <f>SUM(B4,B10,B27)</f>
@@ -4991,20 +5062,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="30.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="1" customWidth="1"/>
-    <col min="2" max="6" width="30.5703125" style="1"/>
-    <col min="7" max="7" width="7.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="30.5703125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="30.5703125" style="1"/>
+    <col min="1" max="1" width="10.1328125" style="1" customWidth="1"/>
+    <col min="2" max="6" width="30.59765625" style="1"/>
+    <col min="7" max="7" width="7.86328125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="30.59765625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="30.59765625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B2" s="21" t="s">
         <v>30</v>
       </c>
@@ -5024,7 +5095,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B3" s="12" t="s">
         <v>36</v>
       </c>
@@ -5044,7 +5115,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B4" s="12" t="s">
         <v>41</v>
       </c>
@@ -5064,7 +5135,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B5" s="12" t="s">
         <v>117</v>
       </c>
@@ -5084,7 +5155,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B6" s="12" t="s">
         <v>99</v>
       </c>
@@ -5104,7 +5175,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B7" s="12" t="s">
         <v>59</v>
       </c>
@@ -5124,7 +5195,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B8" s="12" t="s">
         <v>109</v>
       </c>
@@ -5144,7 +5215,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B9" s="12" t="s">
         <v>71</v>
       </c>
@@ -5164,7 +5235,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B10" s="12" t="s">
         <v>77</v>
       </c>
@@ -5184,7 +5255,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B11" s="12" t="s">
         <v>83</v>
       </c>
@@ -5201,11 +5272,11 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.45">
       <c r="G12"/>
       <c r="H12"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B13" s="24" t="s">
         <v>3</v>
       </c>
@@ -5216,7 +5287,7 @@
         <v>9</v>
       </c>
       <c r="E13" s="27" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F13" s="28" t="s">
         <v>14</v>
@@ -5229,7 +5300,7 @@
       <c r="J13"/>
       <c r="K13"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B14" s="12" t="s">
         <v>89</v>
       </c>
@@ -5253,7 +5324,7 @@
       <c r="J14"/>
       <c r="K14"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B15" s="12" t="s">
         <v>161</v>
       </c>
@@ -5275,7 +5346,7 @@
       <c r="J15"/>
       <c r="K15"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B16" s="12" t="s">
         <v>53</v>
       </c>
@@ -5293,7 +5364,7 @@
       </c>
       <c r="G16"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B17" s="12" t="s">
         <v>119</v>
       </c>
@@ -5320,7 +5391,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B18" s="12" t="s">
         <v>129</v>
       </c>
@@ -5346,7 +5417,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B19" s="12" t="s">
         <v>65</v>
       </c>
@@ -5373,7 +5444,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.45">
       <c r="D20" s="12" t="s">
         <v>149</v>
       </c>
@@ -5388,7 +5459,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
@@ -5404,7 +5475,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B22" s="17" t="s">
         <v>371</v>
       </c>
@@ -5430,7 +5501,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B23" s="12" t="s">
         <v>97</v>
       </c>
@@ -5456,7 +5527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B24" s="12" t="s">
         <v>124</v>
       </c>
@@ -5479,7 +5550,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B25" s="12" t="s">
         <v>114</v>
       </c>
@@ -5495,12 +5566,12 @@
       <c r="F25" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="I25" s="170" t="s">
+      <c r="I25" s="171" t="s">
         <v>370</v>
       </c>
-      <c r="J25" s="170"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J25" s="171"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B26" s="12" t="s">
         <v>134</v>
       </c>
@@ -5516,10 +5587,10 @@
       <c r="F26" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="I26" s="171"/>
-      <c r="J26" s="171"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I26" s="172"/>
+      <c r="J26" s="172"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B27" s="12" t="s">
         <v>144</v>
       </c>
@@ -5536,7 +5607,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B28" s="12" t="s">
         <v>150</v>
       </c>
@@ -5553,15 +5624,15 @@
         <v>147</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.45">
       <c r="F29" s="12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.45">
       <c r="H30"/>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B31" s="11" t="s">
         <v>151</v>
       </c>
@@ -5578,7 +5649,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B32" s="12" t="s">
         <v>139</v>
       </c>
@@ -5595,7 +5666,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B33" s="12" t="s">
         <v>171</v>
       </c>
@@ -5613,7 +5684,7 @@
       </c>
       <c r="H33"/>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B35" s="11" t="s">
         <v>156</v>
       </c>
@@ -5630,7 +5701,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B36" s="12" t="s">
         <v>166</v>
       </c>
@@ -5647,7 +5718,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B37" s="12" t="s">
         <v>176</v>
       </c>
@@ -5664,8 +5735,8 @@
         <v>180</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="39" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B39" s="11" t="s">
         <v>181</v>
       </c>
@@ -5682,7 +5753,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B40" s="12" t="s">
         <v>191</v>
       </c>
@@ -5711,66 +5782,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K70"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="11" width="22.140625" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1328125" style="1"/>
+    <col min="2" max="11" width="22.1328125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" ht="13.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.45">
       <c r="C35"/>
       <c r="D35"/>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.45">
       <c r="C36"/>
       <c r="D36"/>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.45">
       <c r="C37"/>
       <c r="D37"/>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B38" s="172" t="s">
-        <v>484</v>
-      </c>
-      <c r="C38" s="172"/>
-    </row>
-    <row r="40" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B38" s="205" t="s">
+        <v>481</v>
+      </c>
+      <c r="C38" s="205"/>
+    </row>
+    <row r="40" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B40"/>
       <c r="C40"/>
       <c r="D40"/>
       <c r="E40"/>
       <c r="F40"/>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B41" s="177" t="s">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B41" s="195" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="178"/>
-      <c r="D41" s="179" t="s">
+      <c r="C41" s="196"/>
+      <c r="D41" s="197" t="s">
         <v>6</v>
       </c>
-      <c r="E41" s="180"/>
-      <c r="F41" s="181" t="s">
+      <c r="E41" s="198"/>
+      <c r="F41" s="199" t="s">
         <v>9</v>
       </c>
-      <c r="G41" s="182"/>
-      <c r="H41" s="183" t="s">
+      <c r="G41" s="200"/>
+      <c r="H41" s="201" t="s">
         <v>382</v>
       </c>
-      <c r="I41" s="184"/>
-      <c r="J41" s="185" t="s">
+      <c r="I41" s="202"/>
+      <c r="J41" s="203" t="s">
         <v>14</v>
       </c>
-      <c r="K41" s="186"/>
-    </row>
-    <row r="42" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K41" s="204"/>
+    </row>
+    <row r="42" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B42" s="39" t="s">
         <v>30</v>
       </c>
@@ -5802,7 +5873,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B43" s="48" t="s">
         <v>208</v>
       </c>
@@ -5813,7 +5884,7 @@
         <v>210</v>
       </c>
       <c r="E43" s="49" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="F43" s="62" t="s">
         <v>211</v>
@@ -5834,7 +5905,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B44" s="33" t="s">
         <v>217</v>
       </c>
@@ -5854,7 +5925,7 @@
         <v>222</v>
       </c>
       <c r="H44" s="33" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="I44" s="34" t="s">
         <v>223</v>
@@ -5866,87 +5937,87 @@
         <v>225</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B45" s="173" t="s">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B45" s="177" t="s">
         <v>226</v>
       </c>
-      <c r="C45" s="174"/>
-      <c r="D45" s="173" t="s">
+      <c r="C45" s="179"/>
+      <c r="D45" s="177" t="s">
+        <v>467</v>
+      </c>
+      <c r="E45" s="178"/>
+      <c r="F45" s="180" t="s">
+        <v>227</v>
+      </c>
+      <c r="G45" s="179"/>
+      <c r="H45" s="177" t="s">
+        <v>228</v>
+      </c>
+      <c r="I45" s="178"/>
+      <c r="J45" s="180" t="s">
+        <v>229</v>
+      </c>
+      <c r="K45" s="178"/>
+    </row>
+    <row r="46" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B46" s="181" t="s">
+        <v>230</v>
+      </c>
+      <c r="C46" s="183"/>
+      <c r="D46" s="181" t="s">
+        <v>231</v>
+      </c>
+      <c r="E46" s="182"/>
+      <c r="F46" s="184" t="s">
         <v>469</v>
       </c>
-      <c r="E45" s="175"/>
-      <c r="F45" s="176" t="s">
-        <v>227</v>
-      </c>
-      <c r="G45" s="174"/>
-      <c r="H45" s="173" t="s">
-        <v>228</v>
-      </c>
-      <c r="I45" s="175"/>
-      <c r="J45" s="176" t="s">
-        <v>229</v>
-      </c>
-      <c r="K45" s="175"/>
-    </row>
-    <row r="46" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="197" t="s">
-        <v>230</v>
-      </c>
-      <c r="C46" s="198"/>
-      <c r="D46" s="197" t="s">
-        <v>231</v>
-      </c>
-      <c r="E46" s="199"/>
-      <c r="F46" s="200" t="s">
-        <v>471</v>
-      </c>
-      <c r="G46" s="198"/>
-      <c r="H46" s="197" t="s">
-        <v>465</v>
-      </c>
-      <c r="I46" s="199"/>
-      <c r="J46" s="200" t="s">
+      <c r="G46" s="183"/>
+      <c r="H46" s="181" t="s">
+        <v>463</v>
+      </c>
+      <c r="I46" s="182"/>
+      <c r="J46" s="184" t="s">
         <v>232</v>
       </c>
-      <c r="K46" s="199"/>
-    </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K46" s="182"/>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B48"/>
       <c r="C48"/>
       <c r="D48"/>
       <c r="E48"/>
       <c r="F48"/>
     </row>
-    <row r="49" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B49"/>
       <c r="C49"/>
       <c r="D49"/>
       <c r="E49"/>
       <c r="F49"/>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B50" s="187" t="s">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B50" s="185" t="s">
         <v>371</v>
       </c>
-      <c r="C50" s="188"/>
-      <c r="D50" s="189" t="s">
+      <c r="C50" s="186"/>
+      <c r="D50" s="187" t="s">
         <v>23</v>
       </c>
-      <c r="E50" s="190"/>
-      <c r="F50" s="191" t="s">
+      <c r="E50" s="188"/>
+      <c r="F50" s="189" t="s">
         <v>27</v>
       </c>
-      <c r="G50" s="192"/>
-      <c r="H50" s="193" t="s">
+      <c r="G50" s="190"/>
+      <c r="H50" s="191" t="s">
         <v>20</v>
       </c>
-      <c r="I50" s="194"/>
-      <c r="J50" s="195" t="s">
+      <c r="I50" s="192"/>
+      <c r="J50" s="193" t="s">
         <v>17</v>
       </c>
-      <c r="K50" s="196"/>
-    </row>
-    <row r="51" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K50" s="194"/>
+    </row>
+    <row r="51" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B51" s="51" t="s">
         <v>30</v>
       </c>
@@ -5978,12 +6049,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B52" s="31" t="s">
         <v>388</v>
       </c>
       <c r="C52" s="32" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="D52" s="66" t="s">
         <v>236</v>
@@ -6008,12 +6079,12 @@
         <v>233</v>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B53" s="35" t="s">
         <v>249</v>
       </c>
       <c r="C53" s="36" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="D53" s="64" t="s">
         <v>243</v>
@@ -6038,52 +6109,52 @@
         <v>240</v>
       </c>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B54" s="173" t="s">
-        <v>481</v>
-      </c>
-      <c r="C54" s="175"/>
-      <c r="D54" s="176" t="s">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B54" s="177" t="s">
+        <v>478</v>
+      </c>
+      <c r="C54" s="178"/>
+      <c r="D54" s="180" t="s">
         <v>248</v>
       </c>
-      <c r="E54" s="175"/>
-      <c r="F54" s="176" t="s">
+      <c r="E54" s="178"/>
+      <c r="F54" s="180" t="s">
         <v>250</v>
       </c>
-      <c r="G54" s="174"/>
-      <c r="H54" s="173" t="s">
+      <c r="G54" s="179"/>
+      <c r="H54" s="177" t="s">
         <v>247</v>
       </c>
-      <c r="I54" s="174"/>
-      <c r="J54" s="173" t="s">
-        <v>432</v>
-      </c>
-      <c r="K54" s="175"/>
-    </row>
-    <row r="55" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="197" t="s">
+      <c r="I54" s="179"/>
+      <c r="J54" s="177" t="s">
+        <v>430</v>
+      </c>
+      <c r="K54" s="178"/>
+    </row>
+    <row r="55" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B55" s="181" t="s">
         <v>253</v>
       </c>
-      <c r="C55" s="199"/>
-      <c r="D55" s="200" t="s">
+      <c r="C55" s="182"/>
+      <c r="D55" s="184" t="s">
         <v>252</v>
       </c>
-      <c r="E55" s="199"/>
-      <c r="F55" s="200" t="s">
+      <c r="E55" s="182"/>
+      <c r="F55" s="184" t="s">
         <v>254</v>
       </c>
-      <c r="G55" s="198"/>
-      <c r="H55" s="197" t="s">
+      <c r="G55" s="183"/>
+      <c r="H55" s="181" t="s">
         <v>251</v>
       </c>
-      <c r="I55" s="198"/>
-      <c r="J55" s="197" t="s">
-        <v>468</v>
-      </c>
-      <c r="K55" s="199"/>
-    </row>
-    <row r="57" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I55" s="183"/>
+      <c r="J55" s="181" t="s">
+        <v>466</v>
+      </c>
+      <c r="K55" s="182"/>
+    </row>
+    <row r="57" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B58" s="87" t="s">
         <v>258</v>
       </c>
@@ -6094,13 +6165,13 @@
         <v>256</v>
       </c>
       <c r="G58" s="8"/>
-      <c r="I58" s="202" t="s">
+      <c r="I58" s="174" t="s">
         <v>257</v>
       </c>
-      <c r="J58" s="203"/>
-      <c r="K58" s="204"/>
-    </row>
-    <row r="59" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J58" s="175"/>
+      <c r="K58" s="176"/>
+    </row>
+    <row r="59" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B59" s="81" t="s">
         <v>35</v>
       </c>
@@ -6120,9 +6191,9 @@
         <v>261</v>
       </c>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B60" s="69" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="E60" s="31" t="s">
         <v>262</v>
@@ -6140,7 +6211,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B61" s="70" t="s">
         <v>272</v>
       </c>
@@ -6160,7 +6231,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="62" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B62" s="70" t="s">
         <v>278</v>
       </c>
@@ -6180,7 +6251,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="63" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B63" s="71" t="s">
         <v>283</v>
       </c>
@@ -6197,7 +6268,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="64" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E64" s="67" t="s">
         <v>284</v>
       </c>
@@ -6209,28 +6280,52 @@
         <v>286</v>
       </c>
     </row>
-    <row r="65" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="I65" s="80" t="s">
+        <v>532</v>
+      </c>
       <c r="J65" s="71" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="66" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="67" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="67" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B67" s="113" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="68" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B68" s="111" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C70" s="201"/>
-      <c r="D70" s="201"/>
+        <v>430</v>
+      </c>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="C70" s="173"/>
+      <c r="D70" s="173"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="J46:K46"/>
     <mergeCell ref="C70:D70"/>
     <mergeCell ref="I58:K58"/>
     <mergeCell ref="B54:C54"/>
@@ -6243,27 +6338,6 @@
     <mergeCell ref="D55:E55"/>
     <mergeCell ref="J55:K55"/>
     <mergeCell ref="F55:G55"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="H45:I45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -6278,16 +6352,16 @@
       <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="94"/>
-    <col min="2" max="2" width="27.5703125" style="94" customWidth="1"/>
-    <col min="3" max="4" width="58.42578125" style="94" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="94"/>
+    <col min="1" max="1" width="9.1328125" style="94"/>
+    <col min="2" max="2" width="27.59765625" style="94" customWidth="1"/>
+    <col min="3" max="4" width="58.3984375" style="94" customWidth="1"/>
+    <col min="5" max="16384" width="9.1328125" style="94"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="151" t="s">
         <v>288</v>
       </c>
@@ -6298,7 +6372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B4" s="110" t="s">
         <v>290</v>
       </c>
@@ -6309,7 +6383,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B5" s="108" t="s">
         <v>293</v>
       </c>
@@ -6318,98 +6392,98 @@
       </c>
       <c r="D5" s="100"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B6" s="108" t="s">
         <v>295</v>
       </c>
       <c r="C6" s="116"/>
       <c r="D6" s="100"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B7" s="108" t="s">
         <v>296</v>
       </c>
       <c r="C7" s="116" t="s">
         <v>297</v>
       </c>
-      <c r="D7" s="205" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="206" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B8" s="108" t="s">
         <v>298</v>
       </c>
       <c r="C8" s="116" t="s">
         <v>299</v>
       </c>
-      <c r="D8" s="206"/>
-    </row>
-    <row r="9" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D8" s="207"/>
+    </row>
+    <row r="9" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B9" s="108" t="s">
         <v>300</v>
       </c>
       <c r="C9" s="116" t="s">
         <v>301</v>
       </c>
-      <c r="D9" s="206"/>
-    </row>
-    <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D9" s="207"/>
+    </row>
+    <row r="10" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B10" s="108" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C10" s="116" t="s">
         <v>302</v>
       </c>
-      <c r="D10" s="206"/>
-    </row>
-    <row r="11" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D10" s="207"/>
+    </row>
+    <row r="11" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B11" s="108" t="s">
         <v>303</v>
       </c>
       <c r="C11" s="116" t="s">
         <v>304</v>
       </c>
-      <c r="D11" s="206"/>
-    </row>
-    <row r="12" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="D11" s="207"/>
+    </row>
+    <row r="12" spans="2:4" ht="57" x14ac:dyDescent="0.45">
       <c r="B12" s="108" t="s">
         <v>305</v>
       </c>
       <c r="C12" s="116" t="s">
         <v>306</v>
       </c>
-      <c r="D12" s="206"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="207"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B13" s="108" t="s">
         <v>307</v>
       </c>
       <c r="C13" s="116" t="s">
         <v>308</v>
       </c>
-      <c r="D13" s="206"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="207"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B14" s="108" t="s">
         <v>309</v>
       </c>
       <c r="C14" s="116" t="s">
         <v>310</v>
       </c>
-      <c r="D14" s="206"/>
-    </row>
-    <row r="15" spans="2:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="207"/>
+    </row>
+    <row r="15" spans="2:4" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="109" t="s">
         <v>311</v>
       </c>
       <c r="C15" s="114" t="s">
         <v>312</v>
       </c>
-      <c r="D15" s="207"/>
-    </row>
-    <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="208"/>
+    </row>
+    <row r="19" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="20" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B20" s="151" t="s">
         <v>313</v>
       </c>
@@ -6420,7 +6494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B21" s="110" t="s">
         <v>314</v>
       </c>
@@ -6429,7 +6503,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B22" s="108" t="s">
         <v>316</v>
       </c>
@@ -6440,7 +6514,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="108" t="s">
         <v>319</v>
       </c>
@@ -6451,36 +6525,36 @@
         <v>321</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B24" s="108" t="s">
         <v>322</v>
       </c>
       <c r="C24" s="116" t="s">
         <v>323</v>
       </c>
-      <c r="D24" s="205" t="s">
+      <c r="D24" s="206" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="108" t="s">
         <v>325</v>
       </c>
       <c r="C25" s="116" t="s">
         <v>326</v>
       </c>
-      <c r="D25" s="206"/>
-    </row>
-    <row r="26" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D25" s="207"/>
+    </row>
+    <row r="26" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B26" s="108" t="s">
         <v>327</v>
       </c>
       <c r="C26" s="116" t="s">
         <v>328</v>
       </c>
-      <c r="D26" s="209"/>
-    </row>
-    <row r="27" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D26" s="210"/>
+    </row>
+    <row r="27" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B27" s="108" t="s">
         <v>329</v>
       </c>
@@ -6491,7 +6565,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="28" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B28" s="108" t="s">
         <v>332</v>
       </c>
@@ -6502,7 +6576,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B29" s="108" t="s">
         <v>335</v>
       </c>
@@ -6513,7 +6587,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B30" s="108" t="s">
         <v>338</v>
       </c>
@@ -6524,7 +6598,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="31" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B31" s="108" t="s">
         <v>341</v>
       </c>
@@ -6535,7 +6609,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="32" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B32" s="108" t="s">
         <v>290</v>
       </c>
@@ -6546,7 +6620,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="33" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B33" s="109" t="s">
         <v>344</v>
       </c>
@@ -6557,8 +6631,8 @@
         <v>346</v>
       </c>
     </row>
-    <row r="35" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="36" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B36" s="154" t="s">
         <v>347</v>
       </c>
@@ -6569,78 +6643,78 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B37" s="107" t="s">
         <v>348</v>
       </c>
       <c r="C37" s="149" t="s">
         <v>349</v>
       </c>
-      <c r="D37" s="208" t="s">
+      <c r="D37" s="209" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="38" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B38" s="108" t="s">
         <v>351</v>
       </c>
       <c r="C38" s="116" t="s">
         <v>352</v>
       </c>
-      <c r="D38" s="209"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="210"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B39" s="108"/>
       <c r="C39" s="116"/>
       <c r="D39" s="100"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B40" s="108"/>
       <c r="C40" s="116"/>
       <c r="D40" s="100"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B41" s="108"/>
       <c r="C41" s="116"/>
       <c r="D41" s="100"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B42" s="108"/>
       <c r="C42" s="116"/>
       <c r="D42" s="100"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B43" s="108"/>
       <c r="C43" s="116"/>
       <c r="D43" s="100"/>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B44" s="108"/>
       <c r="C44" s="116"/>
       <c r="D44" s="100"/>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B45" s="108"/>
       <c r="C45" s="116"/>
       <c r="D45" s="100"/>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B46" s="108"/>
       <c r="C46" s="116"/>
       <c r="D46" s="100"/>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B47" s="108"/>
       <c r="C47" s="116"/>
       <c r="D47" s="100"/>
     </row>
-    <row r="48" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B48" s="109"/>
       <c r="C48" s="114"/>
       <c r="D48" s="103"/>
     </row>
-    <row r="49" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="50" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B50" s="151" t="s">
         <v>353</v>
       </c>
@@ -6651,35 +6725,35 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B51" s="110" t="s">
         <v>354</v>
       </c>
       <c r="C51" s="149"/>
-      <c r="D51" s="208" t="s">
+      <c r="D51" s="209" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B52" s="108" t="s">
         <v>356</v>
       </c>
       <c r="C52" s="116"/>
-      <c r="D52" s="206"/>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D52" s="207"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B53" s="108" t="s">
         <v>357</v>
       </c>
       <c r="C53" s="116"/>
-      <c r="D53" s="209"/>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D53" s="210"/>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B54" s="108"/>
       <c r="C54" s="116"/>
       <c r="D54" s="100"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B55" s="108" t="s">
         <v>358</v>
       </c>
@@ -6688,14 +6762,14 @@
       </c>
       <c r="D55" s="100"/>
     </row>
-    <row r="56" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B56" s="108"/>
       <c r="C56" s="116" t="s">
         <v>360</v>
       </c>
       <c r="D56" s="100"/>
     </row>
-    <row r="57" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B57" s="108" t="s">
         <v>361</v>
       </c>
@@ -6704,40 +6778,40 @@
       </c>
       <c r="D57" s="100"/>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B58" s="108" t="s">
         <v>363</v>
       </c>
       <c r="C58" s="116"/>
       <c r="D58" s="100"/>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B59" s="108"/>
       <c r="C59" s="116"/>
       <c r="D59" s="100"/>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B60" s="108"/>
       <c r="C60" s="116"/>
       <c r="D60" s="100"/>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B61" s="108"/>
       <c r="C61" s="116"/>
       <c r="D61" s="100"/>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B62" s="108"/>
       <c r="C62" s="116"/>
       <c r="D62" s="100"/>
     </row>
-    <row r="63" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B63" s="109"/>
       <c r="C63" s="114"/>
       <c r="D63" s="103"/>
     </row>
-    <row r="64" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="65" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="65" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B65" s="154" t="s">
         <v>422</v>
       </c>
@@ -6748,152 +6822,152 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B66" s="108" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C66" s="116" t="s">
-        <v>464</v>
-      </c>
-      <c r="D66" s="208" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="67" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D66" s="209" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B67" s="108" t="s">
+        <v>452</v>
+      </c>
+      <c r="C67" s="116" t="s">
+        <v>456</v>
+      </c>
+      <c r="D67" s="207"/>
+    </row>
+    <row r="68" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B68" s="108" t="s">
+        <v>453</v>
+      </c>
+      <c r="C68" s="116" t="s">
+        <v>457</v>
+      </c>
+      <c r="D68" s="207"/>
+    </row>
+    <row r="69" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B69" s="108" t="s">
         <v>454</v>
       </c>
-      <c r="C67" s="116" t="s">
+      <c r="C69" s="116" t="s">
         <v>458</v>
       </c>
-      <c r="D67" s="206"/>
-    </row>
-    <row r="68" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="108" t="s">
+      <c r="D69" s="207"/>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B70" s="108" t="s">
         <v>455</v>
       </c>
-      <c r="C68" s="116" t="s">
+      <c r="C70" s="116" t="s">
         <v>459</v>
       </c>
-      <c r="D68" s="206"/>
-    </row>
-    <row r="69" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B69" s="108" t="s">
-        <v>456</v>
-      </c>
-      <c r="C69" s="116" t="s">
-        <v>460</v>
-      </c>
-      <c r="D69" s="206"/>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B70" s="108" t="s">
-        <v>457</v>
-      </c>
-      <c r="C70" s="116" t="s">
-        <v>461</v>
-      </c>
-      <c r="D70" s="209"/>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D70" s="210"/>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B71" s="108"/>
       <c r="C71" s="116"/>
       <c r="D71" s="100"/>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B72" s="108"/>
       <c r="C72" s="116"/>
       <c r="D72" s="100"/>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B73" s="108"/>
       <c r="C73" s="116"/>
       <c r="D73" s="100"/>
     </row>
-    <row r="74" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B74" s="109"/>
       <c r="C74" s="114"/>
       <c r="D74" s="103"/>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B79" s="95"/>
       <c r="C79" s="95"/>
       <c r="D79" s="95"/>
       <c r="E79" s="95"/>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B80" s="95"/>
       <c r="C80" s="95"/>
-      <c r="D80" s="210"/>
+      <c r="D80" s="211"/>
       <c r="E80" s="95"/>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B81" s="95"/>
       <c r="C81" s="95"/>
-      <c r="D81" s="210"/>
+      <c r="D81" s="211"/>
       <c r="E81" s="95"/>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B82" s="95"/>
       <c r="C82" s="95"/>
-      <c r="D82" s="210"/>
+      <c r="D82" s="211"/>
       <c r="E82" s="95"/>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B83" s="95"/>
       <c r="C83" s="95"/>
       <c r="D83" s="95"/>
       <c r="E83" s="95"/>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B84" s="95"/>
       <c r="C84" s="95"/>
       <c r="D84" s="95"/>
       <c r="E84" s="95"/>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B85" s="95"/>
       <c r="C85" s="95"/>
       <c r="D85" s="95"/>
       <c r="E85" s="95"/>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B86" s="95"/>
       <c r="C86" s="95"/>
       <c r="D86" s="95"/>
       <c r="E86" s="95"/>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B87" s="95"/>
       <c r="C87" s="95"/>
       <c r="D87" s="95"/>
       <c r="E87" s="95"/>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B88" s="95"/>
       <c r="C88" s="95"/>
       <c r="D88" s="95"/>
       <c r="E88" s="95"/>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B89" s="95"/>
       <c r="C89" s="95"/>
       <c r="D89" s="95"/>
       <c r="E89" s="95"/>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B90" s="95"/>
       <c r="C90" s="95"/>
       <c r="D90" s="95"/>
       <c r="E90" s="95"/>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B91" s="95"/>
       <c r="C91" s="95"/>
       <c r="D91" s="95"/>
       <c r="E91" s="95"/>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B92" s="95"/>
       <c r="C92" s="95"/>
       <c r="D92" s="95"/>
@@ -6920,16 +6994,16 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="22.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" customWidth="1"/>
-    <col min="2" max="6" width="22.140625" style="1"/>
-    <col min="7" max="7" width="7.140625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="22.140625" style="1"/>
+    <col min="1" max="1" width="6.59765625" style="1" customWidth="1"/>
+    <col min="2" max="6" width="22.1328125" style="1"/>
+    <col min="7" max="7" width="7.1328125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="22.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="128" t="s">
         <v>30</v>
       </c>
@@ -6949,7 +7023,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B3" s="48"/>
       <c r="C3" s="112"/>
       <c r="D3" s="112"/>
@@ -6959,7 +7033,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B4" s="35"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
@@ -6967,57 +7041,57 @@
       <c r="F4" s="36"/>
       <c r="H4" s="67"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B5" s="35"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="36"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B6" s="35"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="36"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B7" s="35"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="36"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B8" s="35"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="36"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B9" s="35"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="36"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B10" s="35"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="36"/>
     </row>
-    <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="37"/>
       <c r="C11" s="133"/>
       <c r="D11" s="133"/>
       <c r="E11" s="133"/>
       <c r="F11" s="38"/>
     </row>
-    <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="13" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B13" s="134" t="s">
         <v>3</v>
       </c>
@@ -7028,66 +7102,66 @@
         <v>9</v>
       </c>
       <c r="E13" s="137" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F13" s="138" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B14" s="48" t="s">
         <v>368</v>
       </c>
       <c r="C14" s="112" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D14" s="112" t="s">
         <v>365</v>
       </c>
       <c r="E14" s="112" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="F14" s="49" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B15" s="35"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="36"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B16" s="35"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="36"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B17" s="35"/>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
       <c r="F17" s="36"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B18" s="35"/>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="36"/>
     </row>
-    <row r="19" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B19" s="37"/>
       <c r="C19" s="133"/>
       <c r="D19" s="133"/>
       <c r="E19" s="133"/>
       <c r="F19" s="38"/>
     </row>
-    <row r="21" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="22" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B22" s="139" t="s">
         <v>371</v>
       </c>
@@ -7104,60 +7178,60 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B23" s="48" t="s">
         <v>366</v>
       </c>
       <c r="C23" s="112" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D23" s="112" t="s">
         <v>28</v>
       </c>
       <c r="E23" s="112" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="F23" s="49" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B24" s="35"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="36"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B25" s="35"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="36"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B26" s="35"/>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="36"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B27" s="35"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="36"/>
     </row>
-    <row r="28" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B28" s="37"/>
       <c r="C28" s="133"/>
       <c r="D28" s="133"/>
       <c r="E28" s="133"/>
       <c r="F28" s="38"/>
     </row>
-    <row r="30" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="31" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B31" s="144" t="s">
         <v>151</v>
       </c>
@@ -7174,22 +7248,22 @@
         <v>155</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B32" s="48"/>
       <c r="C32" s="112"/>
       <c r="D32" s="112"/>
       <c r="E32" s="112"/>
       <c r="F32" s="49"/>
     </row>
-    <row r="33" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B33" s="37"/>
       <c r="C33" s="133"/>
       <c r="D33" s="133"/>
       <c r="E33" s="133"/>
       <c r="F33" s="38"/>
     </row>
-    <row r="34" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="35" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B35" s="144" t="s">
         <v>156</v>
       </c>
@@ -7206,14 +7280,14 @@
         <v>160</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B36" s="48"/>
       <c r="C36" s="112"/>
       <c r="D36" s="112"/>
       <c r="E36" s="112"/>
       <c r="F36" s="49"/>
     </row>
-    <row r="37" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B37" s="37"/>
       <c r="C37" s="133"/>
       <c r="D37" s="133"/>

</xml_diff>

<commit_message>
Added Demacia, Freljord, and Noxus cards
</commit_message>
<xml_diff>
--- a/DesignDoc.xlsx
+++ b/DesignDoc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4815" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4815" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Factions" sheetId="6" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Instants and Sorceries" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3307,12 +3308,102 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3323,93 +3414,6 @@
     <xf numFmtId="0" fontId="1" fillId="33" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3427,9 +3431,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3728,21 +3729,21 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="95"/>
-    <col min="2" max="2" width="14.73046875" style="95" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="27.73046875" style="95" customWidth="1"/>
-    <col min="6" max="6" width="91.86328125" style="95" customWidth="1"/>
-    <col min="7" max="16384" width="9.1328125" style="95"/>
+    <col min="1" max="1" width="9.140625" style="95"/>
+    <col min="2" max="2" width="14.7109375" style="95" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="27.7109375" style="95" customWidth="1"/>
+    <col min="6" max="6" width="91.85546875" style="95" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="95"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="94"/>
       <c r="B1" s="94"/>
       <c r="C1" s="94"/>
     </row>
-    <row r="2" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="94"/>
       <c r="B2" s="90" t="s">
         <v>369</v>
@@ -3760,7 +3761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="94"/>
       <c r="B3" s="117" t="s">
         <v>3</v>
@@ -3778,7 +3779,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="94"/>
       <c r="B4" s="118" t="s">
         <v>6</v>
@@ -3796,7 +3797,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="94"/>
       <c r="B5" s="119" t="s">
         <v>9</v>
@@ -3814,7 +3815,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="94"/>
       <c r="B6" s="120" t="s">
         <v>11</v>
@@ -3832,7 +3833,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="94"/>
       <c r="B7" s="121" t="s">
         <v>14</v>
@@ -3850,7 +3851,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="94"/>
       <c r="B8" s="122" t="s">
         <v>371</v>
@@ -3868,7 +3869,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="94"/>
       <c r="B9" s="123" t="s">
         <v>23</v>
@@ -3886,7 +3887,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="94"/>
       <c r="B10" s="124" t="s">
         <v>27</v>
@@ -3904,7 +3905,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="94"/>
       <c r="B11" s="125" t="s">
         <v>20</v>
@@ -3922,7 +3923,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="94"/>
       <c r="B12" s="126" t="s">
         <v>17</v>
@@ -3940,7 +3941,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="127" t="s">
         <v>258</v>
       </c>
@@ -3970,17 +3971,17 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.265625" customWidth="1"/>
-    <col min="3" max="5" width="52.3984375" customWidth="1"/>
-    <col min="6" max="7" width="48.3984375" customWidth="1"/>
-    <col min="17" max="18" width="18.265625" customWidth="1"/>
-    <col min="19" max="21" width="48.3984375" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="5" width="52.42578125" customWidth="1"/>
+    <col min="6" max="7" width="48.42578125" customWidth="1"/>
+    <col min="17" max="18" width="18.28515625" customWidth="1"/>
+    <col min="19" max="21" width="48.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="90" t="s">
         <v>427</v>
       </c>
@@ -3994,7 +3995,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="107" t="s">
         <v>419</v>
       </c>
@@ -4008,7 +4009,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="109" t="s">
         <v>422</v>
       </c>
@@ -4022,21 +4023,21 @@
         <v>423</v>
       </c>
     </row>
-    <row r="5" spans="2:5" s="170" customFormat="1" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:5" s="170" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="109" t="s">
         <v>525</v>
       </c>
       <c r="C5" s="106" t="s">
         <v>529</v>
       </c>
-      <c r="D5" s="212" t="s">
+      <c r="D5" s="171" t="s">
         <v>530</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="6" spans="2:5" s="170" customFormat="1" ht="85.9" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:5" s="170" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="109" t="s">
         <v>521</v>
       </c>
@@ -4050,8 +4051,8 @@
         <v>522</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="8" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="90" t="s">
         <v>428</v>
       </c>
@@ -4065,7 +4066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B9" s="107" t="s">
         <v>4</v>
       </c>
@@ -4079,7 +4080,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="108" t="s">
         <v>7</v>
       </c>
@@ -4091,7 +4092,7 @@
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="2:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="108" t="s">
         <v>10</v>
       </c>
@@ -4105,7 +4106,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="108" t="s">
         <v>12</v>
       </c>
@@ -4119,7 +4120,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="108" t="s">
         <v>15</v>
       </c>
@@ -4131,7 +4132,7 @@
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="108" t="s">
         <v>18</v>
       </c>
@@ -4141,7 +4142,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="2:5" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B15" s="108" t="s">
         <v>24</v>
       </c>
@@ -4155,7 +4156,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B16" s="108" t="s">
         <v>28</v>
       </c>
@@ -4165,7 +4166,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B17" s="108" t="s">
         <v>437</v>
       </c>
@@ -4179,7 +4180,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B18" s="108" t="s">
         <v>21</v>
       </c>
@@ -4191,7 +4192,7 @@
       </c>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="85.9" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:5" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="109" t="s">
         <v>431</v>
       </c>
@@ -4205,7 +4206,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="156"/>
       <c r="B21" s="156"/>
       <c r="C21" s="157" t="s">
@@ -4213,7 +4214,7 @@
       </c>
       <c r="D21" s="156"/>
     </row>
-    <row r="22" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="156"/>
       <c r="B22" s="90" t="s">
         <v>427</v>
@@ -4225,7 +4226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="156"/>
       <c r="B23" s="107" t="s">
         <v>471</v>
@@ -4237,7 +4238,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="156"/>
       <c r="B24" s="109" t="s">
         <v>472</v>
@@ -4259,20 +4260,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="16.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="167" customWidth="1"/>
-    <col min="2" max="2" width="12.59765625" style="158" customWidth="1"/>
-    <col min="3" max="18" width="20.1328125" style="158" customWidth="1"/>
-    <col min="19" max="16384" width="16.86328125" style="158"/>
+    <col min="2" max="2" width="12.5703125" style="158" customWidth="1"/>
+    <col min="3" max="18" width="20.140625" style="158" customWidth="1"/>
+    <col min="19" max="16384" width="16.85546875" style="158"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="1:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="168" t="s">
         <v>495</v>
       </c>
@@ -4328,10 +4329,10 @@
         <v>258</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="168"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="168" t="s">
         <v>496</v>
       </c>
@@ -4340,11 +4341,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="169"/>
       <c r="C5" s="163"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="169" t="s">
         <v>502</v>
       </c>
@@ -4367,7 +4368,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="169" t="s">
         <v>516</v>
       </c>
@@ -4408,15 +4409,15 @@
         <v>514</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="169" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="168"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="168" t="s">
         <v>486</v>
       </c>
@@ -4425,10 +4426,10 @@
         <v>428</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="168"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="169" t="s">
         <v>485</v>
       </c>
@@ -4437,7 +4438,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="167" t="s">
         <v>517</v>
       </c>
@@ -4494,7 +4495,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="169" t="s">
         <v>188</v>
       </c>
@@ -4551,10 +4552,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="169"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="169" t="s">
         <v>488</v>
       </c>
@@ -4611,7 +4612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="169" t="s">
         <v>313</v>
       </c>
@@ -4668,7 +4669,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="169" t="s">
         <v>489</v>
       </c>
@@ -4677,7 +4678,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="167" t="s">
         <v>518</v>
       </c>
@@ -4734,7 +4735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="169" t="s">
         <v>490</v>
       </c>
@@ -4791,10 +4792,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="169"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="169" t="s">
         <v>491</v>
       </c>
@@ -4851,10 +4852,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="169"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="169" t="s">
         <v>492</v>
       </c>
@@ -4911,10 +4912,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="169"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="168" t="s">
         <v>487</v>
       </c>
@@ -4923,10 +4924,10 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="168"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="169" t="s">
         <v>493</v>
       </c>
@@ -4983,7 +4984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="169" t="s">
         <v>494</v>
       </c>
@@ -5040,10 +5041,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="169"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="168" t="s">
         <v>519</v>
       </c>
@@ -5066,16 +5067,16 @@
       <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="30.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1328125" style="1" customWidth="1"/>
-    <col min="2" max="6" width="30.59765625" style="1"/>
-    <col min="7" max="7" width="7.86328125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="30.59765625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="30.59765625" style="1"/>
+    <col min="1" max="1" width="10.140625" style="1" customWidth="1"/>
+    <col min="2" max="6" width="30.5703125" style="1"/>
+    <col min="7" max="7" width="7.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="30.5703125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="30.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="21" t="s">
         <v>30</v>
       </c>
@@ -5095,7 +5096,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
         <v>36</v>
       </c>
@@ -5115,7 +5116,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
         <v>41</v>
       </c>
@@ -5135,7 +5136,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>117</v>
       </c>
@@ -5155,7 +5156,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
         <v>99</v>
       </c>
@@ -5175,7 +5176,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
         <v>59</v>
       </c>
@@ -5195,7 +5196,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
         <v>109</v>
       </c>
@@ -5215,7 +5216,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
         <v>71</v>
       </c>
@@ -5235,7 +5236,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
         <v>77</v>
       </c>
@@ -5255,7 +5256,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
         <v>83</v>
       </c>
@@ -5272,11 +5273,11 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G12"/>
       <c r="H12"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="24" t="s">
         <v>3</v>
       </c>
@@ -5300,7 +5301,7 @@
       <c r="J13"/>
       <c r="K13"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
         <v>89</v>
       </c>
@@ -5324,7 +5325,7 @@
       <c r="J14"/>
       <c r="K14"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="12" t="s">
         <v>161</v>
       </c>
@@ -5346,7 +5347,7 @@
       <c r="J15"/>
       <c r="K15"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="12" t="s">
         <v>53</v>
       </c>
@@ -5364,7 +5365,7 @@
       </c>
       <c r="G16"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="12" t="s">
         <v>119</v>
       </c>
@@ -5391,7 +5392,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>129</v>
       </c>
@@ -5417,7 +5418,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
         <v>65</v>
       </c>
@@ -5444,7 +5445,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D20" s="12" t="s">
         <v>149</v>
       </c>
@@ -5459,7 +5460,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
@@ -5475,7 +5476,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="17" t="s">
         <v>371</v>
       </c>
@@ -5501,7 +5502,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="12" t="s">
         <v>97</v>
       </c>
@@ -5527,7 +5528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="12" t="s">
         <v>124</v>
       </c>
@@ -5550,7 +5551,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="12" t="s">
         <v>114</v>
       </c>
@@ -5566,12 +5567,12 @@
       <c r="F25" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="I25" s="171" t="s">
+      <c r="I25" s="172" t="s">
         <v>370</v>
       </c>
-      <c r="J25" s="171"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="J25" s="172"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
         <v>134</v>
       </c>
@@ -5587,10 +5588,10 @@
       <c r="F26" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="I26" s="172"/>
-      <c r="J26" s="172"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="I26" s="173"/>
+      <c r="J26" s="173"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="12" t="s">
         <v>144</v>
       </c>
@@ -5607,7 +5608,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="12" t="s">
         <v>150</v>
       </c>
@@ -5624,15 +5625,15 @@
         <v>147</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F29" s="12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H30"/>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="11" t="s">
         <v>151</v>
       </c>
@@ -5649,7 +5650,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="12" t="s">
         <v>139</v>
       </c>
@@ -5666,7 +5667,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="12" t="s">
         <v>171</v>
       </c>
@@ -5684,7 +5685,7 @@
       </c>
       <c r="H33"/>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="s">
         <v>156</v>
       </c>
@@ -5701,7 +5702,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="12" t="s">
         <v>166</v>
       </c>
@@ -5718,7 +5719,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="12" t="s">
         <v>176</v>
       </c>
@@ -5735,8 +5736,8 @@
         <v>180</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="39" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="11" t="s">
         <v>181</v>
       </c>
@@ -5753,7 +5754,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="12" t="s">
         <v>191</v>
       </c>
@@ -5782,66 +5783,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="1"/>
-    <col min="2" max="11" width="22.1328125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.1328125" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="11" width="22.140625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="13.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C35"/>
       <c r="D35"/>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C36"/>
       <c r="D36"/>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C37"/>
       <c r="D37"/>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B38" s="205" t="s">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="174" t="s">
         <v>481</v>
       </c>
-      <c r="C38" s="205"/>
-    </row>
-    <row r="40" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C38" s="174"/>
+    </row>
+    <row r="40" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40"/>
       <c r="C40"/>
       <c r="D40"/>
       <c r="E40"/>
       <c r="F40"/>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B41" s="195" t="s">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="179" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="196"/>
-      <c r="D41" s="197" t="s">
+      <c r="C41" s="180"/>
+      <c r="D41" s="181" t="s">
         <v>6</v>
       </c>
-      <c r="E41" s="198"/>
-      <c r="F41" s="199" t="s">
+      <c r="E41" s="182"/>
+      <c r="F41" s="183" t="s">
         <v>9</v>
       </c>
-      <c r="G41" s="200"/>
-      <c r="H41" s="201" t="s">
+      <c r="G41" s="184"/>
+      <c r="H41" s="185" t="s">
         <v>382</v>
       </c>
-      <c r="I41" s="202"/>
-      <c r="J41" s="203" t="s">
+      <c r="I41" s="186"/>
+      <c r="J41" s="187" t="s">
         <v>14</v>
       </c>
-      <c r="K41" s="204"/>
-    </row>
-    <row r="42" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="K41" s="188"/>
+    </row>
+    <row r="42" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="39" t="s">
         <v>30</v>
       </c>
@@ -5873,7 +5874,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="48" t="s">
         <v>208</v>
       </c>
@@ -5905,7 +5906,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" s="33" t="s">
         <v>217</v>
       </c>
@@ -5937,87 +5938,87 @@
         <v>225</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B45" s="177" t="s">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="175" t="s">
         <v>226</v>
       </c>
-      <c r="C45" s="179"/>
-      <c r="D45" s="177" t="s">
+      <c r="C45" s="176"/>
+      <c r="D45" s="175" t="s">
         <v>467</v>
       </c>
-      <c r="E45" s="178"/>
-      <c r="F45" s="180" t="s">
+      <c r="E45" s="177"/>
+      <c r="F45" s="178" t="s">
         <v>227</v>
       </c>
-      <c r="G45" s="179"/>
-      <c r="H45" s="177" t="s">
+      <c r="G45" s="176"/>
+      <c r="H45" s="175" t="s">
         <v>228</v>
       </c>
-      <c r="I45" s="178"/>
-      <c r="J45" s="180" t="s">
+      <c r="I45" s="177"/>
+      <c r="J45" s="178" t="s">
         <v>229</v>
       </c>
-      <c r="K45" s="178"/>
-    </row>
-    <row r="46" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B46" s="181" t="s">
+      <c r="K45" s="177"/>
+    </row>
+    <row r="46" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="199" t="s">
         <v>230</v>
       </c>
-      <c r="C46" s="183"/>
-      <c r="D46" s="181" t="s">
+      <c r="C46" s="200"/>
+      <c r="D46" s="199" t="s">
         <v>231</v>
       </c>
-      <c r="E46" s="182"/>
-      <c r="F46" s="184" t="s">
+      <c r="E46" s="201"/>
+      <c r="F46" s="202" t="s">
         <v>469</v>
       </c>
-      <c r="G46" s="183"/>
-      <c r="H46" s="181" t="s">
+      <c r="G46" s="200"/>
+      <c r="H46" s="199" t="s">
         <v>463</v>
       </c>
-      <c r="I46" s="182"/>
-      <c r="J46" s="184" t="s">
+      <c r="I46" s="201"/>
+      <c r="J46" s="202" t="s">
         <v>232</v>
       </c>
-      <c r="K46" s="182"/>
-    </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="K46" s="201"/>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48"/>
       <c r="C48"/>
       <c r="D48"/>
       <c r="E48"/>
       <c r="F48"/>
     </row>
-    <row r="49" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="49" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49"/>
       <c r="C49"/>
       <c r="D49"/>
       <c r="E49"/>
       <c r="F49"/>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B50" s="185" t="s">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B50" s="189" t="s">
         <v>371</v>
       </c>
-      <c r="C50" s="186"/>
-      <c r="D50" s="187" t="s">
+      <c r="C50" s="190"/>
+      <c r="D50" s="191" t="s">
         <v>23</v>
       </c>
-      <c r="E50" s="188"/>
-      <c r="F50" s="189" t="s">
+      <c r="E50" s="192"/>
+      <c r="F50" s="193" t="s">
         <v>27</v>
       </c>
-      <c r="G50" s="190"/>
-      <c r="H50" s="191" t="s">
+      <c r="G50" s="194"/>
+      <c r="H50" s="195" t="s">
         <v>20</v>
       </c>
-      <c r="I50" s="192"/>
-      <c r="J50" s="193" t="s">
+      <c r="I50" s="196"/>
+      <c r="J50" s="197" t="s">
         <v>17</v>
       </c>
-      <c r="K50" s="194"/>
-    </row>
-    <row r="51" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="K50" s="198"/>
+    </row>
+    <row r="51" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="51" t="s">
         <v>30</v>
       </c>
@@ -6049,7 +6050,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" s="31" t="s">
         <v>388</v>
       </c>
@@ -6079,7 +6080,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" s="35" t="s">
         <v>249</v>
       </c>
@@ -6109,52 +6110,52 @@
         <v>240</v>
       </c>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B54" s="177" t="s">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B54" s="175" t="s">
         <v>478</v>
       </c>
-      <c r="C54" s="178"/>
-      <c r="D54" s="180" t="s">
+      <c r="C54" s="177"/>
+      <c r="D54" s="178" t="s">
         <v>248</v>
       </c>
-      <c r="E54" s="178"/>
-      <c r="F54" s="180" t="s">
+      <c r="E54" s="177"/>
+      <c r="F54" s="178" t="s">
         <v>250</v>
       </c>
-      <c r="G54" s="179"/>
-      <c r="H54" s="177" t="s">
+      <c r="G54" s="176"/>
+      <c r="H54" s="175" t="s">
         <v>247</v>
       </c>
-      <c r="I54" s="179"/>
-      <c r="J54" s="177" t="s">
+      <c r="I54" s="176"/>
+      <c r="J54" s="175" t="s">
         <v>430</v>
       </c>
-      <c r="K54" s="178"/>
-    </row>
-    <row r="55" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B55" s="181" t="s">
+      <c r="K54" s="177"/>
+    </row>
+    <row r="55" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="199" t="s">
         <v>253</v>
       </c>
-      <c r="C55" s="182"/>
-      <c r="D55" s="184" t="s">
+      <c r="C55" s="201"/>
+      <c r="D55" s="202" t="s">
         <v>252</v>
       </c>
-      <c r="E55" s="182"/>
-      <c r="F55" s="184" t="s">
+      <c r="E55" s="201"/>
+      <c r="F55" s="202" t="s">
         <v>254</v>
       </c>
-      <c r="G55" s="183"/>
-      <c r="H55" s="181" t="s">
+      <c r="G55" s="200"/>
+      <c r="H55" s="199" t="s">
         <v>251</v>
       </c>
-      <c r="I55" s="183"/>
-      <c r="J55" s="181" t="s">
+      <c r="I55" s="200"/>
+      <c r="J55" s="199" t="s">
         <v>466</v>
       </c>
-      <c r="K55" s="182"/>
-    </row>
-    <row r="57" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="K55" s="201"/>
+    </row>
+    <row r="57" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" s="87" t="s">
         <v>258</v>
       </c>
@@ -6165,13 +6166,13 @@
         <v>256</v>
       </c>
       <c r="G58" s="8"/>
-      <c r="I58" s="174" t="s">
+      <c r="I58" s="204" t="s">
         <v>257</v>
       </c>
-      <c r="J58" s="175"/>
-      <c r="K58" s="176"/>
-    </row>
-    <row r="59" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="J58" s="205"/>
+      <c r="K58" s="206"/>
+    </row>
+    <row r="59" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="81" t="s">
         <v>35</v>
       </c>
@@ -6191,7 +6192,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" s="69" t="s">
         <v>470</v>
       </c>
@@ -6211,7 +6212,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61" s="70" t="s">
         <v>272</v>
       </c>
@@ -6231,7 +6232,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="62" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="62" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="70" t="s">
         <v>278</v>
       </c>
@@ -6251,7 +6252,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="63" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="63" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="71" t="s">
         <v>283</v>
       </c>
@@ -6268,7 +6269,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="64" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E64" s="67" t="s">
         <v>284</v>
       </c>
@@ -6280,7 +6281,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="65" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="65" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I65" s="80" t="s">
         <v>532</v>
       </c>
@@ -6288,44 +6289,23 @@
         <v>287</v>
       </c>
     </row>
-    <row r="66" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="67" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="66" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="67" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="113" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="68" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="68" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="111" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="C70" s="173"/>
-      <c r="D70" s="173"/>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C70" s="203"/>
+      <c r="D70" s="203"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="J46:K46"/>
     <mergeCell ref="C70:D70"/>
     <mergeCell ref="I58:K58"/>
     <mergeCell ref="B54:C54"/>
@@ -6338,6 +6318,27 @@
     <mergeCell ref="D55:E55"/>
     <mergeCell ref="J55:K55"/>
     <mergeCell ref="F55:G55"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H45:I45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -6349,19 +6350,19 @@
   <dimension ref="B2:E92"/>
   <sheetViews>
     <sheetView zoomScale="109" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="94"/>
-    <col min="2" max="2" width="27.59765625" style="94" customWidth="1"/>
-    <col min="3" max="4" width="58.3984375" style="94" customWidth="1"/>
-    <col min="5" max="16384" width="9.1328125" style="94"/>
+    <col min="1" max="1" width="9.140625" style="94"/>
+    <col min="2" max="2" width="27.5703125" style="94" customWidth="1"/>
+    <col min="3" max="4" width="58.42578125" style="94" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="94"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="3" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="151" t="s">
         <v>288</v>
       </c>
@@ -6372,7 +6373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="110" t="s">
         <v>290</v>
       </c>
@@ -6383,7 +6384,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="108" t="s">
         <v>293</v>
       </c>
@@ -6392,98 +6393,98 @@
       </c>
       <c r="D5" s="100"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="108" t="s">
         <v>295</v>
       </c>
       <c r="C6" s="116"/>
       <c r="D6" s="100"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="108" t="s">
         <v>296</v>
       </c>
       <c r="C7" s="116" t="s">
         <v>297</v>
       </c>
-      <c r="D7" s="206" t="s">
+      <c r="D7" s="207" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="108" t="s">
         <v>298</v>
       </c>
       <c r="C8" s="116" t="s">
         <v>299</v>
       </c>
-      <c r="D8" s="207"/>
-    </row>
-    <row r="9" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D8" s="208"/>
+    </row>
+    <row r="9" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="108" t="s">
         <v>300</v>
       </c>
       <c r="C9" s="116" t="s">
         <v>301</v>
       </c>
-      <c r="D9" s="207"/>
-    </row>
-    <row r="10" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D9" s="208"/>
+    </row>
+    <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="108" t="s">
         <v>451</v>
       </c>
       <c r="C10" s="116" t="s">
         <v>302</v>
       </c>
-      <c r="D10" s="207"/>
-    </row>
-    <row r="11" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D10" s="208"/>
+    </row>
+    <row r="11" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="108" t="s">
         <v>303</v>
       </c>
       <c r="C11" s="116" t="s">
         <v>304</v>
       </c>
-      <c r="D11" s="207"/>
-    </row>
-    <row r="12" spans="2:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="D11" s="208"/>
+    </row>
+    <row r="12" spans="2:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B12" s="108" t="s">
         <v>305</v>
       </c>
       <c r="C12" s="116" t="s">
         <v>306</v>
       </c>
-      <c r="D12" s="207"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D12" s="208"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="108" t="s">
         <v>307</v>
       </c>
       <c r="C13" s="116" t="s">
         <v>308</v>
       </c>
-      <c r="D13" s="207"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D13" s="208"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="108" t="s">
         <v>309</v>
       </c>
       <c r="C14" s="116" t="s">
         <v>310</v>
       </c>
-      <c r="D14" s="207"/>
-    </row>
-    <row r="15" spans="2:4" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D14" s="208"/>
+    </row>
+    <row r="15" spans="2:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="109" t="s">
         <v>311</v>
       </c>
       <c r="C15" s="114" t="s">
         <v>312</v>
       </c>
-      <c r="D15" s="208"/>
-    </row>
-    <row r="19" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="20" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D15" s="209"/>
+    </row>
+    <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="151" t="s">
         <v>313</v>
       </c>
@@ -6494,7 +6495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="110" t="s">
         <v>314</v>
       </c>
@@ -6503,7 +6504,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B22" s="108" t="s">
         <v>316</v>
       </c>
@@ -6514,7 +6515,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="108" t="s">
         <v>319</v>
       </c>
@@ -6525,36 +6526,36 @@
         <v>321</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="108" t="s">
         <v>322</v>
       </c>
       <c r="C24" s="116" t="s">
         <v>323</v>
       </c>
-      <c r="D24" s="206" t="s">
+      <c r="D24" s="207" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="108" t="s">
         <v>325</v>
       </c>
       <c r="C25" s="116" t="s">
         <v>326</v>
       </c>
-      <c r="D25" s="207"/>
-    </row>
-    <row r="26" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D25" s="208"/>
+    </row>
+    <row r="26" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="108" t="s">
         <v>327</v>
       </c>
       <c r="C26" s="116" t="s">
         <v>328</v>
       </c>
-      <c r="D26" s="210"/>
-    </row>
-    <row r="27" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D26" s="211"/>
+    </row>
+    <row r="27" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="108" t="s">
         <v>329</v>
       </c>
@@ -6565,7 +6566,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="28" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="108" t="s">
         <v>332</v>
       </c>
@@ -6576,7 +6577,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="108" t="s">
         <v>335</v>
       </c>
@@ -6587,7 +6588,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="108" t="s">
         <v>338</v>
       </c>
@@ -6598,7 +6599,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="31" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B31" s="108" t="s">
         <v>341</v>
       </c>
@@ -6609,7 +6610,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="32" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B32" s="108" t="s">
         <v>290</v>
       </c>
@@ -6620,7 +6621,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="33" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="109" t="s">
         <v>344</v>
       </c>
@@ -6631,8 +6632,8 @@
         <v>346</v>
       </c>
     </row>
-    <row r="35" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="36" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="154" t="s">
         <v>347</v>
       </c>
@@ -6643,78 +6644,78 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" s="107" t="s">
         <v>348</v>
       </c>
       <c r="C37" s="149" t="s">
         <v>349</v>
       </c>
-      <c r="D37" s="209" t="s">
+      <c r="D37" s="210" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="108" t="s">
         <v>351</v>
       </c>
       <c r="C38" s="116" t="s">
         <v>352</v>
       </c>
-      <c r="D38" s="210"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D38" s="211"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="108"/>
       <c r="C39" s="116"/>
       <c r="D39" s="100"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="108"/>
       <c r="C40" s="116"/>
       <c r="D40" s="100"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="108"/>
       <c r="C41" s="116"/>
       <c r="D41" s="100"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="108"/>
       <c r="C42" s="116"/>
       <c r="D42" s="100"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="108"/>
       <c r="C43" s="116"/>
       <c r="D43" s="100"/>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" s="108"/>
       <c r="C44" s="116"/>
       <c r="D44" s="100"/>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="108"/>
       <c r="C45" s="116"/>
       <c r="D45" s="100"/>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="108"/>
       <c r="C46" s="116"/>
       <c r="D46" s="100"/>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" s="108"/>
       <c r="C47" s="116"/>
       <c r="D47" s="100"/>
     </row>
-    <row r="48" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="109"/>
       <c r="C48" s="114"/>
       <c r="D48" s="103"/>
     </row>
-    <row r="49" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="50" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="49" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="151" t="s">
         <v>353</v>
       </c>
@@ -6725,35 +6726,35 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="110" t="s">
         <v>354</v>
       </c>
       <c r="C51" s="149"/>
-      <c r="D51" s="209" t="s">
+      <c r="D51" s="210" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="108" t="s">
         <v>356</v>
       </c>
       <c r="C52" s="116"/>
-      <c r="D52" s="207"/>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D52" s="208"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="108" t="s">
         <v>357</v>
       </c>
       <c r="C53" s="116"/>
-      <c r="D53" s="210"/>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D53" s="211"/>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="108"/>
       <c r="C54" s="116"/>
       <c r="D54" s="100"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="108" t="s">
         <v>358</v>
       </c>
@@ -6762,14 +6763,14 @@
       </c>
       <c r="D55" s="100"/>
     </row>
-    <row r="56" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="56" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B56" s="108"/>
       <c r="C56" s="116" t="s">
         <v>360</v>
       </c>
       <c r="D56" s="100"/>
     </row>
-    <row r="57" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B57" s="108" t="s">
         <v>361</v>
       </c>
@@ -6778,40 +6779,40 @@
       </c>
       <c r="D57" s="100"/>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="108" t="s">
         <v>363</v>
       </c>
       <c r="C58" s="116"/>
       <c r="D58" s="100"/>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="108"/>
       <c r="C59" s="116"/>
       <c r="D59" s="100"/>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="108"/>
       <c r="C60" s="116"/>
       <c r="D60" s="100"/>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="108"/>
       <c r="C61" s="116"/>
       <c r="D61" s="100"/>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="108"/>
       <c r="C62" s="116"/>
       <c r="D62" s="100"/>
     </row>
-    <row r="63" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="63" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="109"/>
       <c r="C63" s="114"/>
       <c r="D63" s="103"/>
     </row>
-    <row r="64" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="65" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="65" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="154" t="s">
         <v>422</v>
       </c>
@@ -6822,152 +6823,152 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="108" t="s">
         <v>461</v>
       </c>
       <c r="C66" s="116" t="s">
         <v>462</v>
       </c>
-      <c r="D66" s="209" t="s">
+      <c r="D66" s="210" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="67" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="67" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B67" s="108" t="s">
         <v>452</v>
       </c>
       <c r="C67" s="116" t="s">
         <v>456</v>
       </c>
-      <c r="D67" s="207"/>
-    </row>
-    <row r="68" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D67" s="208"/>
+    </row>
+    <row r="68" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="108" t="s">
         <v>453</v>
       </c>
       <c r="C68" s="116" t="s">
         <v>457</v>
       </c>
-      <c r="D68" s="207"/>
-    </row>
-    <row r="69" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D68" s="208"/>
+    </row>
+    <row r="69" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B69" s="108" t="s">
         <v>454</v>
       </c>
       <c r="C69" s="116" t="s">
         <v>458</v>
       </c>
-      <c r="D69" s="207"/>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="D69" s="208"/>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="108" t="s">
         <v>455</v>
       </c>
       <c r="C70" s="116" t="s">
         <v>459</v>
       </c>
-      <c r="D70" s="210"/>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="D70" s="211"/>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="108"/>
       <c r="C71" s="116"/>
       <c r="D71" s="100"/>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72" s="108"/>
       <c r="C72" s="116"/>
       <c r="D72" s="100"/>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B73" s="108"/>
       <c r="C73" s="116"/>
       <c r="D73" s="100"/>
     </row>
-    <row r="74" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="74" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="109"/>
       <c r="C74" s="114"/>
       <c r="D74" s="103"/>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B79" s="95"/>
       <c r="C79" s="95"/>
       <c r="D79" s="95"/>
       <c r="E79" s="95"/>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B80" s="95"/>
       <c r="C80" s="95"/>
-      <c r="D80" s="211"/>
+      <c r="D80" s="212"/>
       <c r="E80" s="95"/>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" s="95"/>
       <c r="C81" s="95"/>
-      <c r="D81" s="211"/>
+      <c r="D81" s="212"/>
       <c r="E81" s="95"/>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="95"/>
       <c r="C82" s="95"/>
-      <c r="D82" s="211"/>
+      <c r="D82" s="212"/>
       <c r="E82" s="95"/>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="95"/>
       <c r="C83" s="95"/>
       <c r="D83" s="95"/>
       <c r="E83" s="95"/>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" s="95"/>
       <c r="C84" s="95"/>
       <c r="D84" s="95"/>
       <c r="E84" s="95"/>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85" s="95"/>
       <c r="C85" s="95"/>
       <c r="D85" s="95"/>
       <c r="E85" s="95"/>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B86" s="95"/>
       <c r="C86" s="95"/>
       <c r="D86" s="95"/>
       <c r="E86" s="95"/>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B87" s="95"/>
       <c r="C87" s="95"/>
       <c r="D87" s="95"/>
       <c r="E87" s="95"/>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B88" s="95"/>
       <c r="C88" s="95"/>
       <c r="D88" s="95"/>
       <c r="E88" s="95"/>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B89" s="95"/>
       <c r="C89" s="95"/>
       <c r="D89" s="95"/>
       <c r="E89" s="95"/>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90" s="95"/>
       <c r="C90" s="95"/>
       <c r="D90" s="95"/>
       <c r="E90" s="95"/>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B91" s="95"/>
       <c r="C91" s="95"/>
       <c r="D91" s="95"/>
       <c r="E91" s="95"/>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" s="95"/>
       <c r="C92" s="95"/>
       <c r="D92" s="95"/>
@@ -6994,16 +6995,16 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.59765625" style="1" customWidth="1"/>
-    <col min="2" max="6" width="22.1328125" style="1"/>
-    <col min="7" max="7" width="7.1328125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="22.1328125" style="1"/>
+    <col min="1" max="1" width="6.5703125" style="1" customWidth="1"/>
+    <col min="2" max="6" width="22.140625" style="1"/>
+    <col min="7" max="7" width="7.140625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="22.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="128" t="s">
         <v>30</v>
       </c>
@@ -7023,7 +7024,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="48"/>
       <c r="C3" s="112"/>
       <c r="D3" s="112"/>
@@ -7033,7 +7034,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="35"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
@@ -7041,57 +7042,57 @@
       <c r="F4" s="36"/>
       <c r="H4" s="67"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="35"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="36"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="35"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="36"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="35"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="36"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="35"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="36"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="35"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="36"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="35"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="36"/>
     </row>
-    <row r="11" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="37"/>
       <c r="C11" s="133"/>
       <c r="D11" s="133"/>
       <c r="E11" s="133"/>
       <c r="F11" s="38"/>
     </row>
-    <row r="12" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="13" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="134" t="s">
         <v>3</v>
       </c>
@@ -7108,7 +7109,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="48" t="s">
         <v>368</v>
       </c>
@@ -7125,43 +7126,43 @@
         <v>364</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="35"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="36"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="35"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="36"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="35"/>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
       <c r="F17" s="36"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="35"/>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="36"/>
     </row>
-    <row r="19" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="37"/>
       <c r="C19" s="133"/>
       <c r="D19" s="133"/>
       <c r="E19" s="133"/>
       <c r="F19" s="38"/>
     </row>
-    <row r="21" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="22" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="139" t="s">
         <v>371</v>
       </c>
@@ -7178,7 +7179,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="48" t="s">
         <v>366</v>
       </c>
@@ -7195,43 +7196,43 @@
         <v>445</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="35"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="36"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="35"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="36"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="35"/>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="36"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="35"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="36"/>
     </row>
-    <row r="28" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="37"/>
       <c r="C28" s="133"/>
       <c r="D28" s="133"/>
       <c r="E28" s="133"/>
       <c r="F28" s="38"/>
     </row>
-    <row r="30" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="31" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="144" t="s">
         <v>151</v>
       </c>
@@ -7248,22 +7249,22 @@
         <v>155</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="48"/>
       <c r="C32" s="112"/>
       <c r="D32" s="112"/>
       <c r="E32" s="112"/>
       <c r="F32" s="49"/>
     </row>
-    <row r="33" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="37"/>
       <c r="C33" s="133"/>
       <c r="D33" s="133"/>
       <c r="E33" s="133"/>
       <c r="F33" s="38"/>
     </row>
-    <row r="34" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="35" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="144" t="s">
         <v>156</v>
       </c>
@@ -7280,14 +7281,14 @@
         <v>160</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="48"/>
       <c r="C36" s="112"/>
       <c r="D36" s="112"/>
       <c r="E36" s="112"/>
       <c r="F36" s="49"/>
     </row>
-    <row r="37" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="37"/>
       <c r="C37" s="133"/>
       <c r="D37" s="133"/>

</xml_diff>